<commit_message>
Various updates to make more complete reference set
</commit_message>
<xml_diff>
--- a/tabular/flavi-reference_feature_locations.xlsx
+++ b/tabular/flavi-reference_feature_locations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="27820" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="2360" yWindow="0" windowWidth="26080" windowHeight="26840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="99">
   <si>
     <t>featureName</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>NKV1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Tamanavirus</t>
   </si>
 </sst>
 </file>
@@ -378,7 +384,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,12 +459,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -479,7 +479,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1941">
+  <cellStyleXfs count="1969">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2421,8 +2421,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2457,12 +2485,11 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1941">
+  <cellStyles count="1969">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3434,6 +3461,20 @@
     <cellStyle name="Followed Hyperlink" xfId="1936" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1938" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1940" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1942" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1944" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1946" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1948" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1950" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1952" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1954" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1956" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1958" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1960" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1962" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1964" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1966" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1968" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -4403,6 +4444,20 @@
     <cellStyle name="Hyperlink" xfId="1935" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1937" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1939" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1941" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1943" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1945" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1947" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1949" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1951" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1953" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1955" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1957" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1959" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1961" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1963" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1965" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1967" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4742,8 +4797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1487"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H15" sqref="F3:H15"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H157" sqref="H157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7423,7 +7478,7 @@
       <c r="D104" t="s">
         <v>82</v>
       </c>
-      <c r="E104" s="22" t="s">
+      <c r="E104" s="21" t="s">
         <v>82</v>
       </c>
       <c r="F104" s="9" t="s">
@@ -7449,7 +7504,7 @@
       <c r="D105" t="s">
         <v>82</v>
       </c>
-      <c r="E105" s="22" t="s">
+      <c r="E105" s="21" t="s">
         <v>82</v>
       </c>
       <c r="F105" s="9" t="s">
@@ -7475,7 +7530,7 @@
       <c r="D106" t="s">
         <v>82</v>
       </c>
-      <c r="E106" s="22" t="s">
+      <c r="E106" s="21" t="s">
         <v>82</v>
       </c>
       <c r="F106" s="9" t="s">
@@ -7813,7 +7868,7 @@
       <c r="D120" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E120" s="23" t="s">
+      <c r="E120" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F120" s="9" t="s">
@@ -7839,7 +7894,7 @@
       <c r="D121" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E121" s="23" t="s">
+      <c r="E121" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F121" s="9" t="s">
@@ -7865,7 +7920,7 @@
       <c r="D122" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E122" s="23" t="s">
+      <c r="E122" s="22" t="s">
         <v>94</v>
       </c>
       <c r="F122" s="9" t="s">
@@ -8225,12 +8280,10 @@
         <v>81</v>
       </c>
       <c r="D137" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E137" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="F137" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E137"/>
+      <c r="F137" t="s">
         <v>65</v>
       </c>
       <c r="G137">
@@ -8239,6 +8292,315 @@
       <c r="H137">
         <v>10053</v>
       </c>
+    </row>
+    <row r="138" spans="1:8">
+      <c r="A138" t="s">
+        <v>86</v>
+      </c>
+      <c r="B138" t="s">
+        <v>87</v>
+      </c>
+      <c r="C138" t="s">
+        <v>81</v>
+      </c>
+      <c r="D138" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E138"/>
+      <c r="F138" t="s">
+        <v>21</v>
+      </c>
+      <c r="G138">
+        <v>1</v>
+      </c>
+      <c r="H138">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8">
+      <c r="A139" t="s">
+        <v>86</v>
+      </c>
+      <c r="B139" t="s">
+        <v>87</v>
+      </c>
+      <c r="C139" t="s">
+        <v>81</v>
+      </c>
+      <c r="D139" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E139"/>
+      <c r="F139" t="s">
+        <v>22</v>
+      </c>
+      <c r="G139" s="9">
+        <v>346</v>
+      </c>
+      <c r="H139" s="9">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8">
+      <c r="A140" t="s">
+        <v>86</v>
+      </c>
+      <c r="B140" t="s">
+        <v>87</v>
+      </c>
+      <c r="C140" t="s">
+        <v>81</v>
+      </c>
+      <c r="D140" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E140"/>
+      <c r="F140" t="s">
+        <v>97</v>
+      </c>
+      <c r="G140" s="9">
+        <v>655</v>
+      </c>
+      <c r="H140" s="9">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8">
+      <c r="A141" t="s">
+        <v>86</v>
+      </c>
+      <c r="B141" t="s">
+        <v>87</v>
+      </c>
+      <c r="C141" t="s">
+        <v>81</v>
+      </c>
+      <c r="D141" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E141"/>
+      <c r="F141" t="s">
+        <v>23</v>
+      </c>
+      <c r="G141" s="9">
+        <v>853</v>
+      </c>
+      <c r="H141" s="9">
+        <v>2358</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8">
+      <c r="A142" t="s">
+        <v>86</v>
+      </c>
+      <c r="B142" t="s">
+        <v>87</v>
+      </c>
+      <c r="C142" t="s">
+        <v>81</v>
+      </c>
+      <c r="D142" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E142"/>
+      <c r="F142" t="s">
+        <v>5</v>
+      </c>
+      <c r="G142" s="9">
+        <v>2359</v>
+      </c>
+      <c r="H142" s="9">
+        <v>3390</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8">
+      <c r="A143" t="s">
+        <v>86</v>
+      </c>
+      <c r="B143" t="s">
+        <v>87</v>
+      </c>
+      <c r="C143" t="s">
+        <v>81</v>
+      </c>
+      <c r="D143" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E143"/>
+      <c r="F143" t="s">
+        <v>6</v>
+      </c>
+      <c r="G143" s="9">
+        <v>3391</v>
+      </c>
+      <c r="H143" s="9">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" t="s">
+        <v>87</v>
+      </c>
+      <c r="C144" t="s">
+        <v>81</v>
+      </c>
+      <c r="D144" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E144"/>
+      <c r="F144" t="s">
+        <v>7</v>
+      </c>
+      <c r="G144" s="9">
+        <v>3979</v>
+      </c>
+      <c r="H144" s="9">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" t="s">
+        <v>87</v>
+      </c>
+      <c r="C145" t="s">
+        <v>81</v>
+      </c>
+      <c r="D145" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E145"/>
+      <c r="F145" t="s">
+        <v>8</v>
+      </c>
+      <c r="G145" s="9">
+        <v>4432</v>
+      </c>
+      <c r="H145" s="9">
+        <v>6303</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8">
+      <c r="A146" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" t="s">
+        <v>87</v>
+      </c>
+      <c r="C146" t="s">
+        <v>81</v>
+      </c>
+      <c r="D146" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E146"/>
+      <c r="F146" t="s">
+        <v>9</v>
+      </c>
+      <c r="G146" s="9">
+        <v>6304</v>
+      </c>
+      <c r="H146" s="9">
+        <v>6687</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8">
+      <c r="A147" t="s">
+        <v>86</v>
+      </c>
+      <c r="B147" t="s">
+        <v>87</v>
+      </c>
+      <c r="C147" t="s">
+        <v>81</v>
+      </c>
+      <c r="D147" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E147"/>
+      <c r="F147" t="s">
+        <v>24</v>
+      </c>
+      <c r="G147" s="9">
+        <v>6763</v>
+      </c>
+      <c r="H147" s="9">
+        <v>6762</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8">
+      <c r="A148" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" t="s">
+        <v>87</v>
+      </c>
+      <c r="C148" t="s">
+        <v>81</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E148"/>
+      <c r="F148" t="s">
+        <v>10</v>
+      </c>
+      <c r="G148" s="9">
+        <v>6763</v>
+      </c>
+      <c r="H148" s="9">
+        <v>7557</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8">
+      <c r="A149" t="s">
+        <v>86</v>
+      </c>
+      <c r="B149" t="s">
+        <v>87</v>
+      </c>
+      <c r="C149" t="s">
+        <v>81</v>
+      </c>
+      <c r="D149" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="E149"/>
+      <c r="F149" t="s">
+        <v>11</v>
+      </c>
+      <c r="G149" s="9">
+        <v>7558</v>
+      </c>
+      <c r="H149" s="9">
+        <v>10050</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8">
+      <c r="E150"/>
+    </row>
+    <row r="151" spans="1:8">
+      <c r="E151"/>
+    </row>
+    <row r="152" spans="1:8">
+      <c r="E152"/>
+    </row>
+    <row r="153" spans="1:8">
+      <c r="E153"/>
+    </row>
+    <row r="154" spans="1:8">
+      <c r="E154"/>
+    </row>
+    <row r="155" spans="1:8">
+      <c r="E155"/>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="E156"/>
     </row>
     <row r="198" spans="3:3">
       <c r="C198" s="1"/>

</xml_diff>

<commit_message>
Updated feature locations ids
</commit_message>
<xml_diff>
--- a/tabular/flavi-reference_feature_locations.xlsx
+++ b/tabular/flavi-reference_feature_locations.xlsx
@@ -1,29 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C6656-9EF3-B44C-A732-E184CC646ADF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15660" yWindow="3980" windowWidth="26080" windowHeight="26840" tabRatio="500"/>
+    <workbookView xWindow="12460" yWindow="460" windowWidth="16340" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="694" uniqueCount="86">
   <si>
     <t>featureName</t>
   </si>
@@ -97,12 +103,6 @@
     <t>core</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>p7</t>
   </si>
   <si>
@@ -118,16 +118,7 @@
     <t>Pegivirus</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Pestivirus</t>
-  </si>
-  <si>
-    <t>N-pro</t>
   </si>
   <si>
     <t>RNAse</t>
@@ -223,13 +214,7 @@
     <t>Nematode</t>
   </si>
   <si>
-    <t>NS5-like protein</t>
-  </si>
-  <si>
     <t>NKV1</t>
-  </si>
-  <si>
-    <t>M</t>
   </si>
   <si>
     <t>Tamanavirus</t>
@@ -276,11 +261,38 @@
   <si>
     <t>precursor_polyprotein</t>
   </si>
+  <si>
+    <t>premembrane</t>
+  </si>
+  <si>
+    <t>membrane</t>
+  </si>
+  <si>
+    <t>envelope</t>
+  </si>
+  <si>
+    <t>envelope1</t>
+  </si>
+  <si>
+    <t>envelope2</t>
+  </si>
+  <si>
+    <t>NS5-like</t>
+  </si>
+  <si>
+    <t>s_peptide</t>
+  </si>
+  <si>
+    <t>x_peptide</t>
+  </si>
+  <si>
+    <t>N-proteinase</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4786,14 +4798,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1460"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -4804,18 +4816,18 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -4827,18 +4839,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>16</v>
@@ -4850,21 +4862,21 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F3" s="7">
         <v>97</v>
@@ -4873,21 +4885,21 @@
         <v>10170</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F4" s="7">
         <v>97</v>
@@ -4896,21 +4908,21 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F5" s="7">
         <v>526</v>
@@ -4919,21 +4931,21 @@
         <v>954</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F6" s="7">
         <v>955</v>
@@ -4942,18 +4954,18 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>4</v>
@@ -4965,18 +4977,18 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>5</v>
@@ -4988,18 +5000,18 @@
         <v>4041</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>6</v>
@@ -5011,18 +5023,18 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>7</v>
@@ -5034,18 +5046,18 @@
         <v>6249</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>8</v>
@@ -5057,18 +5069,18 @@
         <v>6654</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>20</v>
@@ -5080,18 +5092,18 @@
         <v>6723</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>9</v>
@@ -5103,18 +5115,18 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>10</v>
@@ -5126,18 +5138,18 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>11</v>
@@ -5149,18 +5161,18 @@
         <v>11375</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>16</v>
@@ -5172,21 +5184,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F17" s="9">
         <v>120</v>
@@ -5195,18 +5207,18 @@
         <v>10445</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>11</v>
@@ -5218,18 +5230,18 @@
         <v>10761</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>16</v>
@@ -5241,21 +5253,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F20" s="9">
         <v>16</v>
@@ -5264,18 +5276,18 @@
         <v>10320</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
         <v>16</v>
@@ -5287,21 +5299,21 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F22">
         <v>95</v>
@@ -5310,21 +5322,21 @@
         <v>10273</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F23">
         <v>95</v>
@@ -5333,21 +5345,21 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F24">
         <v>437</v>
@@ -5356,21 +5368,21 @@
         <v>934</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F25">
         <v>935</v>
@@ -5379,18 +5391,18 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
         <v>4</v>
@@ -5402,18 +5414,18 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
         <v>5</v>
@@ -5425,18 +5437,18 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
         <v>6</v>
@@ -5448,18 +5460,18 @@
         <v>4519</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E29" t="s">
         <v>7</v>
@@ -5471,18 +5483,18 @@
         <v>6376</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -5494,18 +5506,18 @@
         <v>6757</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
         <v>20</v>
@@ -5517,18 +5529,18 @@
         <v>6826</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
         <v>10</v>
@@ -5540,18 +5552,18 @@
         <v>10270</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -5563,18 +5575,18 @@
         <v>10735</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1">
+    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>16</v>
@@ -5586,21 +5598,21 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F35" s="7">
         <v>119</v>
@@ -5609,21 +5621,21 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F36" s="7">
         <v>119</v>
@@ -5632,21 +5644,21 @@
         <v>481</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F37" s="7">
         <v>482</v>
@@ -5655,21 +5667,21 @@
         <v>973</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F38" s="7">
         <v>974</v>
@@ -5678,18 +5690,18 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E39" s="7" t="s">
         <v>4</v>
@@ -5701,18 +5713,18 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>5</v>
@@ -5724,18 +5736,18 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>6</v>
@@ -5747,18 +5759,18 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>7</v>
@@ -5770,18 +5782,18 @@
         <v>6439</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E43" s="7" t="s">
         <v>8</v>
@@ -5793,18 +5805,18 @@
         <v>6817</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E44" s="7" t="s">
         <v>20</v>
@@ -5816,18 +5828,18 @@
         <v>6886</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E45" s="7" t="s">
         <v>9</v>
@@ -5839,18 +5851,18 @@
         <v>7636</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E46" s="7" t="s">
         <v>10</v>
@@ -5862,18 +5874,18 @@
         <v>10351</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>11</v>
@@ -5885,21 +5897,21 @@
         <v>10862</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F48" s="9">
         <v>1</v>
@@ -5908,21 +5920,21 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C49" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -5931,18 +5943,18 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>16</v>
@@ -5954,21 +5966,21 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F51" s="10">
         <v>112</v>
@@ -5977,21 +5989,21 @@
         <v>10359</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E52" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F52" s="9">
         <v>112</v>
@@ -6000,21 +6012,21 @@
         <v>441</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E53" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F53" s="9">
         <v>442</v>
@@ -6023,21 +6035,21 @@
         <v>945</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" t="s">
         <v>79</v>
-      </c>
-      <c r="C54" t="s">
-        <v>15</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E54" t="s">
-        <v>19</v>
       </c>
       <c r="F54" s="9">
         <v>946</v>
@@ -6046,18 +6058,18 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E55" s="9" t="s">
         <v>4</v>
@@ -6069,18 +6081,18 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
       </c>
       <c r="D56" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E56" s="9" t="s">
         <v>5</v>
@@ -6092,18 +6104,18 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E57" s="9" t="s">
         <v>6</v>
@@ -6115,18 +6127,18 @@
         <v>4578</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
       </c>
       <c r="D58" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E58" s="9" t="s">
         <v>7</v>
@@ -6138,18 +6150,18 @@
         <v>6444</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>8</v>
@@ -6161,18 +6173,18 @@
         <v>6822</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E60" s="9" t="s">
         <v>20</v>
@@ -6184,18 +6196,18 @@
         <v>6891</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
       </c>
       <c r="D61" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E61" s="9" t="s">
         <v>9</v>
@@ -6207,18 +6219,18 @@
         <v>7647</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E62" s="9" t="s">
         <v>10</v>
@@ -6230,20 +6242,20 @@
         <v>10356</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E63" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E63" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F63" s="9">
@@ -6253,18 +6265,18 @@
         <v>10839</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C64" t="s">
         <v>22</v>
       </c>
       <c r="D64"/>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F64" s="10">
@@ -6274,19 +6286,19 @@
         <v>341</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C65" t="s">
         <v>22</v>
       </c>
       <c r="D65"/>
-      <c r="E65" s="9" t="s">
-        <v>83</v>
+      <c r="E65" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F65" s="10">
         <v>342</v>
@@ -6295,18 +6307,18 @@
         <v>9377</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
         <v>22</v>
       </c>
       <c r="D66"/>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F66" s="9">
@@ -6316,19 +6328,19 @@
         <v>914</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C67" t="s">
         <v>22</v>
       </c>
       <c r="D67"/>
-      <c r="E67" s="9" t="s">
-        <v>24</v>
+      <c r="E67" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="F67" s="9">
         <v>915</v>
@@ -6337,19 +6349,19 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C68" t="s">
         <v>22</v>
       </c>
       <c r="D68"/>
-      <c r="E68" s="9" t="s">
-        <v>25</v>
+      <c r="E68" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="F68" s="9">
         <v>1491</v>
@@ -6358,19 +6370,19 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C69" t="s">
         <v>22</v>
       </c>
       <c r="D69"/>
-      <c r="E69" s="9" t="s">
-        <v>26</v>
+      <c r="E69" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="F69" s="9">
         <v>2580</v>
@@ -6379,19 +6391,19 @@
         <v>2768</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C70" t="s">
         <v>22</v>
       </c>
       <c r="D70"/>
-      <c r="E70" s="9" t="s">
-        <v>27</v>
+      <c r="E70" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F70" s="9">
         <v>2769</v>
@@ -6400,18 +6412,18 @@
         <v>3419</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C71" t="s">
         <v>22</v>
       </c>
       <c r="D71"/>
-      <c r="E71" s="9" t="s">
+      <c r="E71" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F71" s="9">
@@ -6421,18 +6433,18 @@
         <v>5312</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C72" t="s">
         <v>22</v>
       </c>
       <c r="D72"/>
-      <c r="E72" s="9" t="s">
+      <c r="E72" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F72" s="9">
@@ -6442,18 +6454,18 @@
         <v>5474</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C73" t="s">
         <v>22</v>
       </c>
       <c r="D73"/>
-      <c r="E73" s="9" t="s">
+      <c r="E73" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F73" s="9">
@@ -6463,19 +6475,19 @@
         <v>6257</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
         <v>22</v>
       </c>
       <c r="D74"/>
-      <c r="E74" s="9" t="s">
-        <v>28</v>
+      <c r="E74" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F74" s="9">
         <v>6258</v>
@@ -6484,19 +6496,19 @@
         <v>7601</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C75" t="s">
         <v>22</v>
       </c>
       <c r="D75"/>
-      <c r="E75" s="9" t="s">
-        <v>29</v>
+      <c r="E75" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F75" s="9">
         <v>7602</v>
@@ -6505,18 +6517,18 @@
         <v>9374</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
         <v>22</v>
       </c>
       <c r="D76"/>
-      <c r="E76" s="9" t="s">
+      <c r="E76" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F76" s="9">
@@ -6526,20 +6538,20 @@
         <v>9646</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B77" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C77" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E77" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F77">
@@ -6549,21 +6561,21 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C78" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>66</v>
+        <v>53</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="F78">
         <v>105</v>
@@ -6572,20 +6584,20 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B79" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C79" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="E79" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E79" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F79">
@@ -6595,18 +6607,18 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D80"/>
-      <c r="E80" s="9" t="s">
+      <c r="E80" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F80" s="10">
@@ -6616,19 +6628,19 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81"/>
+      <c r="E81" s="10" t="s">
         <v>76</v>
-      </c>
-      <c r="C81" t="s">
-        <v>30</v>
-      </c>
-      <c r="D81"/>
-      <c r="E81" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="F81" s="10">
         <v>328</v>
@@ -6637,19 +6649,19 @@
         <v>9501</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B82" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C82" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D82"/>
-      <c r="E82" s="9" t="s">
-        <v>31</v>
+      <c r="E82" s="10" t="s">
+        <v>83</v>
       </c>
       <c r="F82" s="9">
         <v>328</v>
@@ -6658,19 +6670,19 @@
         <v>564</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D83"/>
-      <c r="E83" s="9" t="s">
-        <v>24</v>
+      <c r="E83" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="F83" s="9">
         <v>565</v>
@@ -6679,19 +6691,19 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D84"/>
-      <c r="E84" s="9" t="s">
-        <v>25</v>
+      <c r="E84" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="F84" s="9">
         <v>1138</v>
@@ -6700,19 +6712,19 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D85"/>
-      <c r="E85" s="9" t="s">
-        <v>32</v>
+      <c r="E85" s="10" t="s">
+        <v>84</v>
       </c>
       <c r="F85" s="9">
         <v>2200</v>
@@ -6721,19 +6733,19 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C86" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D86"/>
-      <c r="E86" s="9" t="s">
-        <v>27</v>
+      <c r="E86" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F86" s="9">
         <v>2911</v>
@@ -6742,18 +6754,18 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D87"/>
-      <c r="E87" s="9" t="s">
+      <c r="E87" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F87" s="9">
@@ -6763,18 +6775,18 @@
         <v>5514</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C88" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D88"/>
-      <c r="E88" s="9" t="s">
+      <c r="E88" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F88" s="9">
@@ -6784,18 +6796,18 @@
         <v>5637</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C89" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D89"/>
-      <c r="E89" s="9" t="s">
+      <c r="E89" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F89" s="9">
@@ -6805,19 +6817,19 @@
         <v>6423</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B90" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C90" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D90"/>
-      <c r="E90" s="9" t="s">
-        <v>28</v>
+      <c r="E90" s="10" t="s">
+        <v>26</v>
       </c>
       <c r="F90" s="9">
         <v>6424</v>
@@ -6826,19 +6838,19 @@
         <v>7797</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B91" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C91" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D91"/>
-      <c r="E91" s="9" t="s">
-        <v>29</v>
+      <c r="E91" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="F91" s="9">
         <v>7798</v>
@@ -6847,18 +6859,18 @@
         <v>9498</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B92" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C92" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D92"/>
-      <c r="E92" s="9" t="s">
+      <c r="E92" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F92" s="9">
@@ -6868,20 +6880,20 @@
         <v>9867</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B93" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C93" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D93" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E93" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E93" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F93">
@@ -6891,21 +6903,21 @@
         <v>350</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B94" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D94" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>83</v>
+        <v>60</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F94">
         <v>351</v>
@@ -6914,20 +6926,20 @@
         <v>18068</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B95" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C95" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D95" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="E95" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E95" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F95">
@@ -6937,18 +6949,18 @@
         <v>19199</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C96" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D96"/>
-      <c r="E96" s="9" t="s">
+      <c r="E96" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F96" s="10">
@@ -6958,19 +6970,19 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B97" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C97" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D97"/>
-      <c r="E97" s="9" t="s">
-        <v>83</v>
+      <c r="E97" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="F97" s="10">
         <v>386</v>
@@ -6979,19 +6991,19 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C98" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D98"/>
-      <c r="E98" s="9" t="s">
-        <v>34</v>
+      <c r="E98" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="F98" s="9">
         <v>386</v>
@@ -7000,18 +7012,18 @@
         <v>889</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B99" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D99"/>
-      <c r="E99" s="9" t="s">
+      <c r="E99" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F99" s="9">
@@ -7021,19 +7033,19 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B100" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C100" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D100"/>
-      <c r="E100" s="9" t="s">
-        <v>35</v>
+      <c r="E100" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="F100" s="9">
         <v>1196</v>
@@ -7042,19 +7054,19 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C101" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D101"/>
-      <c r="E101" s="9" t="s">
-        <v>24</v>
+      <c r="E101" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="F101" s="9">
         <v>1877</v>
@@ -7063,19 +7075,19 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B102" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D102"/>
-      <c r="E102" s="9" t="s">
-        <v>25</v>
+      <c r="E102" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="F102" s="9">
         <v>2462</v>
@@ -7084,19 +7096,19 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C103" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D103"/>
-      <c r="E103" s="9" t="s">
-        <v>26</v>
+      <c r="E103" s="10" t="s">
+        <v>24</v>
       </c>
       <c r="F103" s="9">
         <v>3584</v>
@@ -7105,18 +7117,18 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B104" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C104" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D104"/>
-      <c r="E104" s="9" t="s">
+      <c r="E104" s="10" t="s">
         <v>7</v>
       </c>
       <c r="F104" s="9">
@@ -7126,18 +7138,18 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B105" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D105"/>
-      <c r="E105" s="9" t="s">
+      <c r="E105" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F105" s="9">
@@ -7147,18 +7159,18 @@
         <v>7663</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B106" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C106" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D106"/>
-      <c r="E106" s="9" t="s">
+      <c r="E106" s="10" t="s">
         <v>9</v>
       </c>
       <c r="F106" s="9">
@@ -7168,19 +7180,19 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B107" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C107" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D107"/>
       <c r="E107" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F107" s="9">
         <v>8705</v>
@@ -7189,19 +7201,19 @@
         <v>10192</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B108" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C108" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D108"/>
       <c r="E108" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F108" s="9">
         <v>10193</v>
@@ -7210,15 +7222,15 @@
         <v>12349</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C109" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D109"/>
       <c r="E109" s="9" t="s">
@@ -7231,19 +7243,19 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B110" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D110"/>
       <c r="E110" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -7252,19 +7264,19 @@
         <v>10053</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B111" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D111"/>
       <c r="E111" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -7273,19 +7285,19 @@
         <v>345</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B112" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D112"/>
       <c r="E112" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="F112" s="9">
         <v>346</v>
@@ -7294,19 +7306,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B113" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D113"/>
       <c r="E113" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="F113" s="9">
         <v>655</v>
@@ -7315,19 +7327,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B114" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D114"/>
       <c r="E114" t="s">
-        <v>19</v>
+        <v>79</v>
       </c>
       <c r="F114" s="9">
         <v>853</v>
@@ -7336,15 +7348,15 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B115" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D115"/>
       <c r="E115" t="s">
@@ -7357,15 +7369,15 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B116" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D116"/>
       <c r="E116" t="s">
@@ -7378,15 +7390,15 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B117" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D117"/>
       <c r="E117" t="s">
@@ -7399,15 +7411,15 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B118" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D118"/>
       <c r="E118" t="s">
@@ -7420,15 +7432,15 @@
         <v>6303</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B119" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D119"/>
       <c r="E119" t="s">
@@ -7441,15 +7453,15 @@
         <v>6687</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B120" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D120"/>
       <c r="E120" t="s">
@@ -7462,15 +7474,15 @@
         <v>6762</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B121" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D121"/>
       <c r="E121" t="s">
@@ -7483,15 +7495,15 @@
         <v>7557</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B122" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D122"/>
       <c r="E122" t="s">
@@ -7504,356 +7516,356 @@
         <v>10050</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D123"/>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D124"/>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D125"/>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D126"/>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D127"/>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D128"/>
     </row>
-    <row r="129" spans="4:4">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D129"/>
     </row>
-    <row r="182" spans="2:4">
+    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B182" s="1"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
     </row>
-    <row r="183" spans="2:4">
+    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B183" s="1"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
     </row>
-    <row r="184" spans="2:4">
+    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B184" s="1"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
     </row>
-    <row r="185" spans="2:4">
+    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B185" s="1"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
     </row>
-    <row r="186" spans="2:4">
+    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B186" s="1"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
     </row>
-    <row r="187" spans="2:4">
+    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B187" s="1"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
     </row>
-    <row r="188" spans="2:4">
+    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B188" s="1"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="2:4">
+    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B189" s="1"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="2:4">
+    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B190" s="1"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="2:4">
+    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B191" s="1"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="2:4">
+    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B192" s="1"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="2:4">
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="1"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="1"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="2:4">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="1"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="2:4">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="1"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="2:4">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="1"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="2:4">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="1"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="2:4">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="1"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="2:4">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="1"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="2:4">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="1"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="1"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="2:4">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="1"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="2:4">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="1"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="2:4">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="1"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="2:4">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="1"/>
     </row>
-    <row r="207" spans="2:4">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="1"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="2:4">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="1"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="2:4">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="1"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="2:4">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="1"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="2:4">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="1"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="2:4">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="1"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="2:4">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="1"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="896" spans="5:5">
+    <row r="896" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E896" s="1"/>
     </row>
-    <row r="1032" spans="2:2">
+    <row r="1032" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1032" s="1"/>
     </row>
-    <row r="1033" spans="2:2">
+    <row r="1033" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1033" s="1"/>
     </row>
-    <row r="1158" spans="2:2">
+    <row r="1158" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1158" s="1"/>
     </row>
-    <row r="1159" spans="2:2">
+    <row r="1159" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1159" s="1"/>
     </row>
-    <row r="1160" spans="2:2">
+    <row r="1160" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1160" s="1"/>
     </row>
-    <row r="1161" spans="2:2">
+    <row r="1161" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1161" s="1"/>
     </row>
-    <row r="1162" spans="2:2">
+    <row r="1162" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1162" s="1"/>
     </row>
-    <row r="1163" spans="2:2">
+    <row r="1163" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1163" s="1"/>
     </row>
-    <row r="1208" spans="2:6">
+    <row r="1208" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1208" s="1"/>
       <c r="F1208" s="1"/>
     </row>
-    <row r="1209" spans="2:6">
+    <row r="1209" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1209" s="1"/>
       <c r="F1209" s="1"/>
     </row>
-    <row r="1210" spans="2:6">
+    <row r="1210" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1210" s="1"/>
       <c r="F1210" s="1"/>
     </row>
-    <row r="1212" spans="2:6">
+    <row r="1212" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1212" s="1"/>
     </row>
-    <row r="1213" spans="2:6">
+    <row r="1213" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1213" s="1"/>
     </row>
-    <row r="1214" spans="2:6">
+    <row r="1214" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1214" s="1"/>
     </row>
-    <row r="1215" spans="2:6">
+    <row r="1215" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1215" s="1"/>
     </row>
-    <row r="1216" spans="2:6">
+    <row r="1216" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1216" s="1"/>
     </row>
-    <row r="1235" spans="2:2">
+    <row r="1235" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1235" s="1"/>
     </row>
-    <row r="1236" spans="2:2">
+    <row r="1236" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1236" s="1"/>
     </row>
-    <row r="1237" spans="2:2">
+    <row r="1237" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1237" s="1"/>
     </row>
-    <row r="1238" spans="2:2">
+    <row r="1238" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1238" s="1"/>
     </row>
-    <row r="1239" spans="2:2">
+    <row r="1239" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1239" s="1"/>
     </row>
-    <row r="1240" spans="2:2">
+    <row r="1240" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1240" s="1"/>
     </row>
-    <row r="1241" spans="2:2">
+    <row r="1241" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1241" s="1"/>
     </row>
-    <row r="1243" spans="2:2">
+    <row r="1243" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1243" s="1"/>
     </row>
-    <row r="1244" spans="2:2">
+    <row r="1244" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1244" s="1"/>
     </row>
-    <row r="1245" spans="2:2">
+    <row r="1245" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1245" s="1"/>
     </row>
-    <row r="1246" spans="2:2">
+    <row r="1246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1246" s="1"/>
     </row>
-    <row r="1247" spans="2:2">
+    <row r="1247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1247" s="1"/>
     </row>
-    <row r="1248" spans="2:2">
+    <row r="1248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1248" s="1"/>
     </row>
-    <row r="1300" spans="2:2">
+    <row r="1300" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1300" s="1"/>
     </row>
-    <row r="1301" spans="2:2">
+    <row r="1301" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1301" s="1"/>
     </row>
-    <row r="1302" spans="2:2">
+    <row r="1302" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1302" s="1"/>
     </row>
-    <row r="1303" spans="2:2">
+    <row r="1303" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1303" s="1"/>
     </row>
-    <row r="1305" spans="2:2">
+    <row r="1305" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1305" s="1"/>
     </row>
-    <row r="1306" spans="2:2">
+    <row r="1306" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1306" s="1"/>
     </row>
-    <row r="1307" spans="2:2">
+    <row r="1307" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1307" s="1"/>
     </row>
-    <row r="1308" spans="2:2">
+    <row r="1308" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1308" s="1"/>
     </row>
-    <row r="1343" spans="2:2">
+    <row r="1343" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1343" s="1"/>
     </row>
-    <row r="1344" spans="2:2">
+    <row r="1344" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1344" s="1"/>
     </row>
-    <row r="1345" spans="2:2">
+    <row r="1345" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1345" s="1"/>
     </row>
-    <row r="1346" spans="2:2">
+    <row r="1346" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1346" s="1"/>
     </row>
-    <row r="1347" spans="2:2">
+    <row r="1347" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1347" s="1"/>
     </row>
-    <row r="1348" spans="2:2">
+    <row r="1348" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1348" s="1"/>
     </row>
-    <row r="1390" spans="3:6">
+    <row r="1390" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1390" s="1"/>
       <c r="F1390" s="1"/>
     </row>
-    <row r="1391" spans="3:6">
+    <row r="1391" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1391" s="6"/>
       <c r="D1391" s="6"/>
       <c r="E1391" s="1"/>
       <c r="F1391" s="1"/>
     </row>
-    <row r="1392" spans="3:6">
+    <row r="1392" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1392" s="6"/>
       <c r="D1392" s="6"/>
       <c r="E1392" s="1"/>
       <c r="F1392" s="1"/>
     </row>
-    <row r="1393" spans="3:6">
+    <row r="1393" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1393" s="6"/>
       <c r="D1393" s="6"/>
       <c r="E1393" s="1"/>
       <c r="F1393" s="1"/>
     </row>
-    <row r="1394" spans="3:6">
+    <row r="1394" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1394" s="1"/>
       <c r="F1394" s="1"/>
     </row>
-    <row r="1457" spans="2:2">
+    <row r="1457" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1457" s="1"/>
     </row>
-    <row r="1458" spans="2:2">
+    <row r="1458" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1458" s="1"/>
     </row>
-    <row r="1459" spans="2:2">
+    <row r="1459" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1459" s="1"/>
     </row>
-    <row r="1460" spans="2:2">
+    <row r="1460" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1460" s="1"/>
     </row>
   </sheetData>
@@ -7872,18 +7884,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -7892,7 +7904,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>16</v>
@@ -7904,9 +7916,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
@@ -7915,10 +7927,10 @@
         <v>15</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F2" s="7">
         <v>97</v>
@@ -7927,9 +7939,9 @@
         <v>10389</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -7938,7 +7950,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>17</v>
@@ -7950,9 +7962,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -7961,7 +7973,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>18</v>
@@ -7973,9 +7985,9 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -7984,7 +7996,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>19</v>
@@ -7996,9 +8008,9 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -8007,7 +8019,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>4</v>
@@ -8019,9 +8031,9 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -8030,7 +8042,7 @@
         <v>15</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E7" s="7" t="s">
         <v>5</v>
@@ -8042,9 +8054,9 @@
         <v>4206</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -8053,7 +8065,7 @@
         <v>15</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>6</v>
@@ -8065,9 +8077,9 @@
         <v>4599</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
@@ -8076,7 +8088,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>7</v>
@@ -8088,9 +8100,9 @@
         <v>6456</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
@@ -8099,7 +8111,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>20</v>
@@ -8111,9 +8123,9 @@
         <v>6903</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
@@ -8122,7 +8134,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>9</v>
@@ -8134,9 +8146,9 @@
         <v>7671</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
@@ -8145,7 +8157,7 @@
         <v>15</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>10</v>
@@ -8157,9 +8169,9 @@
         <v>10386</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
@@ -8168,7 +8180,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>11</v>
@@ -8180,9 +8192,9 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -8191,7 +8203,7 @@
         <v>15</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E14" t="s">
         <v>16</v>
@@ -8203,9 +8215,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>21</v>
@@ -8214,10 +8226,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F15">
         <v>107</v>
@@ -8226,9 +8238,9 @@
         <v>10366</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
         <v>21</v>
@@ -8237,7 +8249,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
         <v>17</v>
@@ -8249,9 +8261,9 @@
         <v>472</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
         <v>21</v>
@@ -8260,7 +8272,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
         <v>18</v>
@@ -8272,9 +8284,9 @@
         <v>976</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
@@ -8283,7 +8295,7 @@
         <v>15</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
@@ -8295,9 +8307,9 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
@@ -8306,7 +8318,7 @@
         <v>15</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
@@ -8318,9 +8330,9 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
         <v>21</v>
@@ -8329,7 +8341,7 @@
         <v>15</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
         <v>5</v>
@@ -8341,9 +8353,9 @@
         <v>4210</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" customHeight="1">
+    <row r="21" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -8352,7 +8364,7 @@
         <v>15</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
         <v>6</v>
@@ -8364,9 +8376,9 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -8375,7 +8387,7 @@
         <v>15</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E22" t="s">
         <v>7</v>
@@ -8387,9 +8399,9 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -8398,7 +8410,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -8410,9 +8422,9 @@
         <v>6832</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
@@ -8421,7 +8433,7 @@
         <v>15</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
@@ -8433,9 +8445,9 @@
         <v>6901</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
@@ -8444,7 +8456,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E25" t="s">
         <v>9</v>
@@ -8456,9 +8468,9 @@
         <v>7654</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -8467,7 +8479,7 @@
         <v>15</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E26" t="s">
         <v>10</v>
@@ -8479,9 +8491,9 @@
         <v>10363</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
@@ -8490,7 +8502,7 @@
         <v>15</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added features and feature locations to reference sequences
</commit_message>
<xml_diff>
--- a/tabular/flavi-reference_feature_locations.xlsx
+++ b/tabular/flavi-reference_feature_locations.xlsx
@@ -1,28 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11014"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus-group/Flaviviridae-GLUE/tabular/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC0C6656-9EF3-B44C-A732-E184CC646ADF}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12460" yWindow="460" windowWidth="16340" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10000" yWindow="0" windowWidth="25360" windowHeight="18100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000"/>
+  <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -172,16 +166,10 @@
     <t>NC_024806</t>
   </si>
   <si>
-    <t>Lammi virus</t>
-  </si>
-  <si>
     <t>dISF2</t>
   </si>
   <si>
     <t>NC_027999</t>
-  </si>
-  <si>
-    <t>Paraiso Escondido virus</t>
   </si>
   <si>
     <t>dISF1</t>
@@ -256,9 +244,6 @@
     <t>REF_APOIV</t>
   </si>
   <si>
-    <t>REF_YFV</t>
-  </si>
-  <si>
     <t>precursor_polyprotein</t>
   </si>
   <si>
@@ -288,11 +273,20 @@
   <si>
     <t>N-proteinase</t>
   </si>
+  <si>
+    <t>REF_EPEV</t>
+  </si>
+  <si>
+    <t>REF_LAMV</t>
+  </si>
+  <si>
+    <t>REF_MASTER_YFV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -447,9 +441,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1987">
+  <cellStyleXfs count="1997">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2475,7 +2479,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1987">
+  <cellStyles count="1997">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -3470,6 +3474,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1982" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1984" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1996" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -4462,6 +4471,11 @@
     <cellStyle name="Hyperlink" xfId="1981" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1983" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1995" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4798,14 +4812,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C30" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E101" sqref="E101"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F47" sqref="A34:F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -4816,12 +4830,12 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>13</v>
@@ -4839,12 +4853,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>15</v>
@@ -4862,12 +4876,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>15</v>
@@ -4876,7 +4890,7 @@
         <v>44</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F3" s="7">
         <v>97</v>
@@ -4885,12 +4899,12 @@
         <v>10170</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>15</v>
@@ -4908,12 +4922,12 @@
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>15</v>
@@ -4922,7 +4936,7 @@
         <v>44</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F5" s="7">
         <v>526</v>
@@ -4931,12 +4945,12 @@
         <v>954</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>15</v>
@@ -4945,7 +4959,7 @@
         <v>44</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F6" s="7">
         <v>955</v>
@@ -4954,12 +4968,12 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>15</v>
@@ -4977,12 +4991,12 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>15</v>
@@ -5000,12 +5014,12 @@
         <v>4041</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>15</v>
@@ -5023,12 +5037,12 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>15</v>
@@ -5046,12 +5060,12 @@
         <v>6249</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>15</v>
@@ -5069,12 +5083,12 @@
         <v>6654</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>15</v>
@@ -5092,12 +5106,12 @@
         <v>6723</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>15</v>
@@ -5115,12 +5129,12 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>15</v>
@@ -5138,12 +5152,12 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>15</v>
@@ -5161,18 +5175,18 @@
         <v>11375</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>16</v>
@@ -5184,21 +5198,21 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>51</v>
-      </c>
       <c r="E17" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F17" s="9">
         <v>120</v>
@@ -5207,18 +5221,18 @@
         <v>10445</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>51</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>11</v>
@@ -5230,18 +5244,18 @@
         <v>10761</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>48</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>16</v>
@@ -5253,21 +5267,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>46</v>
       </c>
       <c r="B20" t="s">
+        <v>84</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>48</v>
-      </c>
       <c r="E20" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F20" s="9">
         <v>16</v>
@@ -5276,12 +5290,12 @@
         <v>10320</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C21" t="s">
         <v>15</v>
@@ -5299,12 +5313,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
         <v>15</v>
@@ -5313,7 +5327,7 @@
         <v>41</v>
       </c>
       <c r="E22" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F22">
         <v>95</v>
@@ -5322,12 +5336,12 @@
         <v>10273</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C23" t="s">
         <v>15</v>
@@ -5345,12 +5359,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
         <v>15</v>
@@ -5359,7 +5373,7 @@
         <v>41</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F24">
         <v>437</v>
@@ -5368,12 +5382,12 @@
         <v>934</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
         <v>15</v>
@@ -5382,7 +5396,7 @@
         <v>41</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F25">
         <v>935</v>
@@ -5391,12 +5405,12 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
@@ -5414,12 +5428,12 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s">
         <v>15</v>
@@ -5437,12 +5451,12 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
@@ -5460,12 +5474,12 @@
         <v>4519</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
         <v>15</v>
@@ -5483,12 +5497,12 @@
         <v>6376</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
         <v>15</v>
@@ -5506,12 +5520,12 @@
         <v>6757</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C31" t="s">
         <v>15</v>
@@ -5529,12 +5543,12 @@
         <v>6826</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C32" t="s">
         <v>15</v>
@@ -5552,12 +5566,12 @@
         <v>10270</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C33" t="s">
         <v>15</v>
@@ -5575,12 +5589,12 @@
         <v>10735</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="16" customHeight="1">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>15</v>
@@ -5598,12 +5612,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>15</v>
@@ -5612,7 +5626,7 @@
         <v>43</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F35" s="7">
         <v>119</v>
@@ -5621,12 +5635,12 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>15</v>
@@ -5644,12 +5658,12 @@
         <v>481</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>15</v>
@@ -5658,7 +5672,7 @@
         <v>43</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F37" s="7">
         <v>482</v>
@@ -5667,12 +5681,12 @@
         <v>973</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>15</v>
@@ -5681,7 +5695,7 @@
         <v>43</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F38" s="7">
         <v>974</v>
@@ -5690,12 +5704,12 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>15</v>
@@ -5713,12 +5727,12 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>15</v>
@@ -5736,12 +5750,12 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>15</v>
@@ -5759,12 +5773,12 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>32</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>15</v>
@@ -5782,12 +5796,12 @@
         <v>6439</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>15</v>
@@ -5805,12 +5819,12 @@
         <v>6817</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>32</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>15</v>
@@ -5828,12 +5842,12 @@
         <v>6886</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>32</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C45" s="7" t="s">
         <v>15</v>
@@ -5851,12 +5865,12 @@
         <v>7636</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>32</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>15</v>
@@ -5874,12 +5888,12 @@
         <v>10351</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>15</v>
@@ -5897,21 +5911,21 @@
         <v>10862</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C48" s="16" t="s">
         <v>15</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F48" s="9">
         <v>1</v>
@@ -5920,21 +5934,21 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="C49" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>76</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -5943,12 +5957,12 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>35</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
@@ -5966,12 +5980,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>35</v>
       </c>
       <c r="B51" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
@@ -5980,7 +5994,7 @@
         <v>45</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F51" s="10">
         <v>112</v>
@@ -5989,12 +6003,12 @@
         <v>10359</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
@@ -6012,12 +6026,12 @@
         <v>441</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
         <v>15</v>
@@ -6026,7 +6040,7 @@
         <v>45</v>
       </c>
       <c r="E53" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F53" s="9">
         <v>442</v>
@@ -6035,12 +6049,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
         <v>15</v>
@@ -6049,7 +6063,7 @@
         <v>45</v>
       </c>
       <c r="E54" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F54" s="9">
         <v>946</v>
@@ -6058,12 +6072,12 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
         <v>15</v>
@@ -6081,12 +6095,12 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C56" t="s">
         <v>15</v>
@@ -6104,12 +6118,12 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>35</v>
       </c>
       <c r="B57" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C57" t="s">
         <v>15</v>
@@ -6127,12 +6141,12 @@
         <v>4578</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
         <v>15</v>
@@ -6150,12 +6164,12 @@
         <v>6444</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>35</v>
       </c>
       <c r="B59" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C59" t="s">
         <v>15</v>
@@ -6173,12 +6187,12 @@
         <v>6822</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>35</v>
       </c>
       <c r="B60" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C60" t="s">
         <v>15</v>
@@ -6196,12 +6210,12 @@
         <v>6891</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>35</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C61" t="s">
         <v>15</v>
@@ -6219,12 +6233,12 @@
         <v>7647</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C62" t="s">
         <v>15</v>
@@ -6242,12 +6256,12 @@
         <v>10356</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
         <v>15</v>
@@ -6265,12 +6279,12 @@
         <v>10839</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>36</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s">
         <v>22</v>
@@ -6286,19 +6300,19 @@
         <v>341</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>36</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
         <v>22</v>
       </c>
       <c r="D65"/>
       <c r="E65" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F65" s="10">
         <v>342</v>
@@ -6307,12 +6321,12 @@
         <v>9377</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C66" t="s">
         <v>22</v>
@@ -6328,19 +6342,19 @@
         <v>914</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
         <v>22</v>
       </c>
       <c r="D67"/>
       <c r="E67" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F67" s="9">
         <v>915</v>
@@ -6349,19 +6363,19 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C68" t="s">
         <v>22</v>
       </c>
       <c r="D68"/>
       <c r="E68" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F68" s="9">
         <v>1491</v>
@@ -6370,12 +6384,12 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C69" t="s">
         <v>22</v>
@@ -6391,12 +6405,12 @@
         <v>2768</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s">
         <v>22</v>
@@ -6412,12 +6426,12 @@
         <v>3419</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>36</v>
       </c>
       <c r="B71" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C71" t="s">
         <v>22</v>
@@ -6433,12 +6447,12 @@
         <v>5312</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>36</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
         <v>22</v>
@@ -6454,12 +6468,12 @@
         <v>5474</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>36</v>
       </c>
       <c r="B73" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C73" t="s">
         <v>22</v>
@@ -6475,12 +6489,12 @@
         <v>6257</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
         <v>22</v>
@@ -6496,12 +6510,12 @@
         <v>7601</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>36</v>
       </c>
       <c r="B75" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C75" t="s">
         <v>22</v>
@@ -6517,12 +6531,12 @@
         <v>9374</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>36</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" t="s">
         <v>22</v>
@@ -6538,18 +6552,18 @@
         <v>9646</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C77" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E77" s="10" t="s">
         <v>16</v>
@@ -6561,21 +6575,21 @@
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C78" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F78">
         <v>105</v>
@@ -6584,18 +6598,18 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B79" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>11</v>
@@ -6607,12 +6621,12 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C80" t="s">
         <v>28</v>
@@ -6628,19 +6642,19 @@
         <v>327</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C81" t="s">
         <v>28</v>
       </c>
       <c r="D81"/>
       <c r="E81" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F81" s="10">
         <v>328</v>
@@ -6649,19 +6663,19 @@
         <v>9501</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>39</v>
       </c>
       <c r="B82" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C82" t="s">
         <v>28</v>
       </c>
       <c r="D82"/>
       <c r="E82" s="10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F82" s="9">
         <v>328</v>
@@ -6670,19 +6684,19 @@
         <v>564</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>39</v>
       </c>
       <c r="B83" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C83" t="s">
         <v>28</v>
       </c>
       <c r="D83"/>
       <c r="E83" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F83" s="9">
         <v>565</v>
@@ -6691,19 +6705,19 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>39</v>
       </c>
       <c r="B84" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C84" t="s">
         <v>28</v>
       </c>
       <c r="D84"/>
       <c r="E84" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F84" s="9">
         <v>1138</v>
@@ -6712,19 +6726,19 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>39</v>
       </c>
       <c r="B85" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C85" t="s">
         <v>28</v>
       </c>
       <c r="D85"/>
       <c r="E85" s="10" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F85" s="9">
         <v>2200</v>
@@ -6733,12 +6747,12 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>39</v>
       </c>
       <c r="B86" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C86" t="s">
         <v>28</v>
@@ -6754,12 +6768,12 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>39</v>
       </c>
       <c r="B87" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C87" t="s">
         <v>28</v>
@@ -6775,12 +6789,12 @@
         <v>5514</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>39</v>
       </c>
       <c r="B88" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C88" t="s">
         <v>28</v>
@@ -6796,12 +6810,12 @@
         <v>5637</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>39</v>
       </c>
       <c r="B89" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C89" t="s">
         <v>28</v>
@@ -6817,12 +6831,12 @@
         <v>6423</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>39</v>
       </c>
       <c r="B90" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C90" t="s">
         <v>28</v>
@@ -6838,12 +6852,12 @@
         <v>7797</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>39</v>
       </c>
       <c r="B91" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C91" t="s">
         <v>28</v>
@@ -6859,12 +6873,12 @@
         <v>9498</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>39</v>
       </c>
       <c r="B92" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C92" t="s">
         <v>28</v>
@@ -6880,18 +6894,18 @@
         <v>9867</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
+        <v>56</v>
+      </c>
+      <c r="B93" t="s">
+        <v>66</v>
+      </c>
+      <c r="C93" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D93" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="B93" t="s">
-        <v>68</v>
-      </c>
-      <c r="C93" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D93" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="E93" s="10" t="s">
         <v>16</v>
@@ -6903,21 +6917,21 @@
         <v>350</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
+        <v>56</v>
+      </c>
+      <c r="B94" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D94" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B94" t="s">
-        <v>68</v>
-      </c>
-      <c r="C94" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D94" s="22" t="s">
-        <v>60</v>
-      </c>
       <c r="E94" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F94">
         <v>351</v>
@@ -6926,18 +6940,18 @@
         <v>18068</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
+        <v>56</v>
+      </c>
+      <c r="B95" t="s">
+        <v>66</v>
+      </c>
+      <c r="C95" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D95" s="22" t="s">
         <v>58</v>
-      </c>
-      <c r="B95" t="s">
-        <v>68</v>
-      </c>
-      <c r="C95" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D95" s="22" t="s">
-        <v>60</v>
       </c>
       <c r="E95" s="10" t="s">
         <v>11</v>
@@ -6949,12 +6963,12 @@
         <v>19199</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>37</v>
       </c>
       <c r="B96" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C96" t="s">
         <v>29</v>
@@ -6970,19 +6984,19 @@
         <v>385</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>37</v>
       </c>
       <c r="B97" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C97" t="s">
         <v>29</v>
       </c>
       <c r="D97"/>
       <c r="E97" s="10" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F97" s="10">
         <v>386</v>
@@ -6991,19 +7005,19 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>37</v>
       </c>
       <c r="B98" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C98" t="s">
         <v>29</v>
       </c>
       <c r="D98"/>
       <c r="E98" s="10" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F98" s="9">
         <v>386</v>
@@ -7012,12 +7026,12 @@
         <v>889</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>37</v>
       </c>
       <c r="B99" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C99" t="s">
         <v>29</v>
@@ -7033,12 +7047,12 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>37</v>
       </c>
       <c r="B100" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C100" t="s">
         <v>29</v>
@@ -7054,19 +7068,19 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>37</v>
       </c>
       <c r="B101" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C101" t="s">
         <v>29</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F101" s="9">
         <v>1877</v>
@@ -7075,19 +7089,19 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:7">
       <c r="A102" t="s">
         <v>37</v>
       </c>
       <c r="B102" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C102" t="s">
         <v>29</v>
       </c>
       <c r="D102"/>
       <c r="E102" s="10" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F102" s="9">
         <v>2462</v>
@@ -7096,12 +7110,12 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:7">
       <c r="A103" t="s">
         <v>37</v>
       </c>
       <c r="B103" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C103" t="s">
         <v>29</v>
@@ -7117,12 +7131,12 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:7">
       <c r="A104" t="s">
         <v>37</v>
       </c>
       <c r="B104" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C104" t="s">
         <v>29</v>
@@ -7138,12 +7152,12 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:7">
       <c r="A105" t="s">
         <v>37</v>
       </c>
       <c r="B105" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C105" t="s">
         <v>29</v>
@@ -7159,12 +7173,12 @@
         <v>7663</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:7">
       <c r="A106" t="s">
         <v>37</v>
       </c>
       <c r="B106" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C106" t="s">
         <v>29</v>
@@ -7180,12 +7194,12 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:7">
       <c r="A107" t="s">
         <v>37</v>
       </c>
       <c r="B107" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C107" t="s">
         <v>29</v>
@@ -7201,12 +7215,12 @@
         <v>10192</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:7">
       <c r="A108" t="s">
         <v>37</v>
       </c>
       <c r="B108" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C108" t="s">
         <v>29</v>
@@ -7222,12 +7236,12 @@
         <v>12349</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7">
       <c r="A109" t="s">
         <v>37</v>
       </c>
       <c r="B109" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C109" t="s">
         <v>29</v>
@@ -7243,19 +7257,19 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B110" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C110" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D110"/>
       <c r="E110" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -7264,15 +7278,15 @@
         <v>10053</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B111" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C111" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D111"/>
       <c r="E111" t="s">
@@ -7285,19 +7299,19 @@
         <v>345</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B112" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C112" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D112"/>
       <c r="E112" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F112" s="9">
         <v>346</v>
@@ -7306,19 +7320,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B113" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C113" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D113"/>
       <c r="E113" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F113" s="9">
         <v>655</v>
@@ -7327,19 +7341,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B114" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C114" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D114"/>
       <c r="E114" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F114" s="9">
         <v>853</v>
@@ -7348,15 +7362,15 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B115" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C115" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D115"/>
       <c r="E115" t="s">
@@ -7369,15 +7383,15 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B116" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D116"/>
       <c r="E116" t="s">
@@ -7390,15 +7404,15 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C117" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D117"/>
       <c r="E117" t="s">
@@ -7411,15 +7425,15 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B118" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C118" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D118"/>
       <c r="E118" t="s">
@@ -7432,15 +7446,15 @@
         <v>6303</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:7">
       <c r="A119" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B119" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C119" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D119"/>
       <c r="E119" t="s">
@@ -7453,36 +7467,36 @@
         <v>6687</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:7">
       <c r="A120" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B120" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C120" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D120"/>
       <c r="E120" t="s">
         <v>20</v>
       </c>
       <c r="F120" s="9">
-        <v>6763</v>
+        <v>6688</v>
       </c>
       <c r="G120" s="9">
         <v>6762</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:7">
       <c r="A121" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B121" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C121" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D121"/>
       <c r="E121" t="s">
@@ -7495,15 +7509,15 @@
         <v>7557</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:7">
       <c r="A122" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B122" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C122" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D122"/>
       <c r="E122" t="s">
@@ -7516,356 +7530,356 @@
         <v>10050</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:7">
       <c r="D123"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:7">
       <c r="D124"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:7">
       <c r="D125"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:7">
       <c r="D126"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:7">
       <c r="D127"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:7">
       <c r="D128"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:4">
       <c r="D129"/>
     </row>
-    <row r="182" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:4">
       <c r="B182" s="1"/>
       <c r="C182" s="5"/>
       <c r="D182" s="5"/>
     </row>
-    <row r="183" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:4">
       <c r="B183" s="1"/>
       <c r="C183" s="5"/>
       <c r="D183" s="5"/>
     </row>
-    <row r="184" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:4">
       <c r="B184" s="1"/>
       <c r="C184" s="5"/>
       <c r="D184" s="5"/>
     </row>
-    <row r="185" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:4">
       <c r="B185" s="1"/>
       <c r="C185" s="5"/>
       <c r="D185" s="5"/>
     </row>
-    <row r="186" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:4">
       <c r="B186" s="1"/>
       <c r="C186" s="5"/>
       <c r="D186" s="5"/>
     </row>
-    <row r="187" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:4">
       <c r="B187" s="1"/>
       <c r="C187" s="5"/>
       <c r="D187" s="5"/>
     </row>
-    <row r="188" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:4">
       <c r="B188" s="1"/>
       <c r="C188" s="5"/>
       <c r="D188" s="5"/>
     </row>
-    <row r="189" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:4">
       <c r="B189" s="1"/>
       <c r="C189" s="5"/>
       <c r="D189" s="5"/>
     </row>
-    <row r="190" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:4">
       <c r="B190" s="1"/>
       <c r="C190" s="5"/>
       <c r="D190" s="5"/>
     </row>
-    <row r="191" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:4">
       <c r="B191" s="1"/>
       <c r="C191" s="5"/>
       <c r="D191" s="5"/>
     </row>
-    <row r="192" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:4">
       <c r="B192" s="1"/>
       <c r="C192" s="5"/>
       <c r="D192" s="5"/>
     </row>
-    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:4">
       <c r="B193" s="1"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:4">
       <c r="B194" s="1"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:4">
       <c r="B195" s="1"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:4">
       <c r="B196" s="1"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:4">
       <c r="B197" s="1"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:4">
       <c r="B198" s="1"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:4">
       <c r="B199" s="1"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:4">
       <c r="B200" s="1"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:4">
       <c r="B201" s="1"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:4">
       <c r="B202" s="1"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:4">
       <c r="B203" s="1"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:4">
       <c r="B204" s="1"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:4">
       <c r="B205" s="1"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:4">
       <c r="B206" s="1"/>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:4">
       <c r="B207" s="1"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:4">
       <c r="B208" s="1"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:4">
       <c r="B209" s="1"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:4">
       <c r="B210" s="1"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:4">
       <c r="B211" s="1"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:4">
       <c r="B212" s="1"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:4">
       <c r="B213" s="1"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="896" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="896" spans="5:5">
       <c r="E896" s="1"/>
     </row>
-    <row r="1032" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1032" spans="2:2">
       <c r="B1032" s="1"/>
     </row>
-    <row r="1033" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1033" spans="2:2">
       <c r="B1033" s="1"/>
     </row>
-    <row r="1158" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1158" spans="2:2">
       <c r="B1158" s="1"/>
     </row>
-    <row r="1159" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1159" spans="2:2">
       <c r="B1159" s="1"/>
     </row>
-    <row r="1160" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1160" spans="2:2">
       <c r="B1160" s="1"/>
     </row>
-    <row r="1161" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1161" spans="2:2">
       <c r="B1161" s="1"/>
     </row>
-    <row r="1162" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1162" spans="2:2">
       <c r="B1162" s="1"/>
     </row>
-    <row r="1163" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1163" spans="2:2">
       <c r="B1163" s="1"/>
     </row>
-    <row r="1208" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1208" spans="2:6">
       <c r="E1208" s="1"/>
       <c r="F1208" s="1"/>
     </row>
-    <row r="1209" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1209" spans="2:6">
       <c r="E1209" s="1"/>
       <c r="F1209" s="1"/>
     </row>
-    <row r="1210" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1210" spans="2:6">
       <c r="E1210" s="1"/>
       <c r="F1210" s="1"/>
     </row>
-    <row r="1212" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1212" spans="2:6">
       <c r="B1212" s="1"/>
     </row>
-    <row r="1213" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1213" spans="2:6">
       <c r="B1213" s="1"/>
     </row>
-    <row r="1214" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1214" spans="2:6">
       <c r="B1214" s="1"/>
     </row>
-    <row r="1215" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1215" spans="2:6">
       <c r="B1215" s="1"/>
     </row>
-    <row r="1216" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="1216" spans="2:6">
       <c r="B1216" s="1"/>
     </row>
-    <row r="1235" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1235" spans="2:2">
       <c r="B1235" s="1"/>
     </row>
-    <row r="1236" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1236" spans="2:2">
       <c r="B1236" s="1"/>
     </row>
-    <row r="1237" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1237" spans="2:2">
       <c r="B1237" s="1"/>
     </row>
-    <row r="1238" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1238" spans="2:2">
       <c r="B1238" s="1"/>
     </row>
-    <row r="1239" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1239" spans="2:2">
       <c r="B1239" s="1"/>
     </row>
-    <row r="1240" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1240" spans="2:2">
       <c r="B1240" s="1"/>
     </row>
-    <row r="1241" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1241" spans="2:2">
       <c r="B1241" s="1"/>
     </row>
-    <row r="1243" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1243" spans="2:2">
       <c r="B1243" s="1"/>
     </row>
-    <row r="1244" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1244" spans="2:2">
       <c r="B1244" s="1"/>
     </row>
-    <row r="1245" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1245" spans="2:2">
       <c r="B1245" s="1"/>
     </row>
-    <row r="1246" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1246" spans="2:2">
       <c r="B1246" s="1"/>
     </row>
-    <row r="1247" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1247" spans="2:2">
       <c r="B1247" s="1"/>
     </row>
-    <row r="1248" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1248" spans="2:2">
       <c r="B1248" s="1"/>
     </row>
-    <row r="1300" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1300" spans="2:2">
       <c r="B1300" s="1"/>
     </row>
-    <row r="1301" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1301" spans="2:2">
       <c r="B1301" s="1"/>
     </row>
-    <row r="1302" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1302" spans="2:2">
       <c r="B1302" s="1"/>
     </row>
-    <row r="1303" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1303" spans="2:2">
       <c r="B1303" s="1"/>
     </row>
-    <row r="1305" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1305" spans="2:2">
       <c r="B1305" s="1"/>
     </row>
-    <row r="1306" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1306" spans="2:2">
       <c r="B1306" s="1"/>
     </row>
-    <row r="1307" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1307" spans="2:2">
       <c r="B1307" s="1"/>
     </row>
-    <row r="1308" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1308" spans="2:2">
       <c r="B1308" s="1"/>
     </row>
-    <row r="1343" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1343" spans="2:2">
       <c r="B1343" s="1"/>
     </row>
-    <row r="1344" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1344" spans="2:2">
       <c r="B1344" s="1"/>
     </row>
-    <row r="1345" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1345" spans="2:2">
       <c r="B1345" s="1"/>
     </row>
-    <row r="1346" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1346" spans="2:2">
       <c r="B1346" s="1"/>
     </row>
-    <row r="1347" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1347" spans="2:2">
       <c r="B1347" s="1"/>
     </row>
-    <row r="1348" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1348" spans="2:2">
       <c r="B1348" s="1"/>
     </row>
-    <row r="1390" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="1390" spans="3:6">
       <c r="E1390" s="1"/>
       <c r="F1390" s="1"/>
     </row>
-    <row r="1391" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="1391" spans="3:6">
       <c r="C1391" s="6"/>
       <c r="D1391" s="6"/>
       <c r="E1391" s="1"/>
       <c r="F1391" s="1"/>
     </row>
-    <row r="1392" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="1392" spans="3:6">
       <c r="C1392" s="6"/>
       <c r="D1392" s="6"/>
       <c r="E1392" s="1"/>
       <c r="F1392" s="1"/>
     </row>
-    <row r="1393" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="1393" spans="3:6">
       <c r="C1393" s="6"/>
       <c r="D1393" s="6"/>
       <c r="E1393" s="1"/>
       <c r="F1393" s="1"/>
     </row>
-    <row r="1394" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="1394" spans="3:6">
       <c r="E1394" s="1"/>
       <c r="F1394" s="1"/>
     </row>
-    <row r="1457" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1457" spans="2:2">
       <c r="B1457" s="1"/>
     </row>
-    <row r="1458" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1458" spans="2:2">
       <c r="B1458" s="1"/>
     </row>
-    <row r="1459" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1459" spans="2:2">
       <c r="B1459" s="1"/>
     </row>
-    <row r="1460" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="1460" spans="2:2">
       <c r="B1460" s="1"/>
     </row>
   </sheetData>
@@ -7884,16 +7898,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -7916,7 +7930,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -7939,7 +7953,7 @@
         <v>10389</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -7962,7 +7976,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -7985,7 +7999,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -8008,7 +8022,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -8031,7 +8045,7 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -8054,7 +8068,7 @@
         <v>4206</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -8077,7 +8091,7 @@
         <v>4599</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -8100,7 +8114,7 @@
         <v>6456</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -8123,7 +8137,7 @@
         <v>6903</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -8146,7 +8160,7 @@
         <v>7671</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -8169,7 +8183,7 @@
         <v>10386</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -8192,7 +8206,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -8215,7 +8229,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -8238,7 +8252,7 @@
         <v>10366</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -8261,7 +8275,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -8284,7 +8298,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -8307,7 +8321,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -8330,7 +8344,7 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -8353,7 +8367,7 @@
         <v>4210</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="14" customHeight="1">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -8376,7 +8390,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -8399,7 +8413,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -8422,7 +8436,7 @@
         <v>6832</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -8445,7 +8459,7 @@
         <v>6901</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -8468,7 +8482,7 @@
         <v>7654</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -8491,7 +8505,7 @@
         <v>10363</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Added feature locations for Jingmenviruses
</commit_message>
<xml_diff>
--- a/tabular/flavi-reference_feature_locations.xlsx
+++ b/tabular/flavi-reference_feature_locations.xlsx
@@ -1,29 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Projects/virus/comparative/Flaviviridae-GLUE/tabular/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3D408-F9B8-044B-B0E9-E74A60FAA18D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17220" yWindow="0" windowWidth="25300" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="460" windowWidth="28060" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="926" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="115">
   <si>
     <t>featureName</t>
   </si>
@@ -193,9 +199,6 @@
     <t>Pesti-like</t>
   </si>
   <si>
-    <t>Nematode</t>
-  </si>
-  <si>
     <t>NKV1</t>
   </si>
   <si>
@@ -350,12 +353,33 @@
   </si>
   <si>
     <t>Primate</t>
+  </si>
+  <si>
+    <t>NC_024113</t>
+  </si>
+  <si>
+    <t>Jingmenvirus</t>
+  </si>
+  <si>
+    <t>PL1</t>
+  </si>
+  <si>
+    <t>PL2</t>
+  </si>
+  <si>
+    <t>Human-Tick</t>
+  </si>
+  <si>
+    <t>NC_024114</t>
+  </si>
+  <si>
+    <t>REF_JMTV_SEG3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -5499,14 +5523,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1471"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
@@ -5517,12 +5541,12 @@
     <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>12</v>
@@ -5540,12 +5564,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="37" t="s">
         <v>14</v>
@@ -5554,7 +5578,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="7">
         <v>1</v>
@@ -5563,12 +5587,12 @@
         <v>11375</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" s="37" t="s">
         <v>14</v>
@@ -5586,12 +5610,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C4" s="37" t="s">
         <v>14</v>
@@ -5600,7 +5624,7 @@
         <v>42</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F4" s="7">
         <v>97</v>
@@ -5609,12 +5633,12 @@
         <v>10170</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="37" t="s">
         <v>14</v>
@@ -5623,7 +5647,7 @@
         <v>42</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="7">
         <v>97</v>
@@ -5632,12 +5656,12 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="37" t="s">
         <v>14</v>
@@ -5646,7 +5670,7 @@
         <v>42</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F6" s="7">
         <v>97</v>
@@ -5655,12 +5679,12 @@
         <v>525</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="37" t="s">
         <v>14</v>
@@ -5669,7 +5693,7 @@
         <v>42</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F7" s="7">
         <v>526</v>
@@ -5678,12 +5702,12 @@
         <v>954</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="37" t="s">
         <v>14</v>
@@ -5692,7 +5716,7 @@
         <v>42</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="7">
         <v>955</v>
@@ -5701,12 +5725,12 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>14</v>
@@ -5715,7 +5739,7 @@
         <v>42</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F9" s="7">
         <v>2251</v>
@@ -5724,12 +5748,12 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="37" t="s">
         <v>14</v>
@@ -5747,12 +5771,12 @@
         <v>3420</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="37" t="s">
         <v>14</v>
@@ -5761,7 +5785,7 @@
         <v>42</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F11" s="7">
         <v>3421</v>
@@ -5770,12 +5794,12 @@
         <v>4041</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="37" t="s">
         <v>14</v>
@@ -5784,7 +5808,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="7">
         <v>4042</v>
@@ -5793,12 +5817,12 @@
         <v>4488</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C13" s="37" t="s">
         <v>14</v>
@@ -5816,12 +5840,12 @@
         <v>6249</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="37" t="s">
         <v>14</v>
@@ -5830,7 +5854,7 @@
         <v>42</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F14" s="7">
         <v>6250</v>
@@ -5839,12 +5863,12 @@
         <v>6654</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="37" t="s">
         <v>14</v>
@@ -5862,12 +5886,12 @@
         <v>6723</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="37" t="s">
         <v>14</v>
@@ -5876,7 +5900,7 @@
         <v>42</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F16" s="7">
         <v>6724</v>
@@ -5885,12 +5909,12 @@
         <v>7503</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="37" t="s">
         <v>14</v>
@@ -5908,12 +5932,12 @@
         <v>10167</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="37" t="s">
         <v>14</v>
@@ -5931,12 +5955,12 @@
         <v>11375</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="38" t="s">
         <v>14</v>
@@ -5945,7 +5969,7 @@
         <v>47</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F19" s="26">
         <v>1</v>
@@ -5954,12 +5978,12 @@
         <v>10761</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="38" t="s">
         <v>14</v>
@@ -5977,12 +6001,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C21" s="38" t="s">
         <v>14</v>
@@ -5991,7 +6015,7 @@
         <v>47</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F21" s="26">
         <v>120</v>
@@ -6000,12 +6024,12 @@
         <v>10445</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B22" s="36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C22" s="38" t="s">
         <v>14</v>
@@ -6023,12 +6047,12 @@
         <v>10761</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="38" t="s">
         <v>14</v>
@@ -6037,7 +6061,7 @@
         <v>45</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F23" s="26">
         <v>1</v>
@@ -6046,12 +6070,12 @@
         <v>10320</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C24" s="38" t="s">
         <v>14</v>
@@ -6069,12 +6093,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" s="38" t="s">
         <v>14</v>
@@ -6083,7 +6107,7 @@
         <v>45</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F25" s="26">
         <v>16</v>
@@ -6092,12 +6116,12 @@
         <v>10320</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C26" s="36" t="s">
         <v>14</v>
@@ -6106,7 +6130,7 @@
         <v>39</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F26" s="28">
         <v>1</v>
@@ -6115,12 +6139,12 @@
         <v>10735</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B27" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="36" t="s">
         <v>14</v>
@@ -6138,12 +6162,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="36" t="s">
         <v>14</v>
@@ -6152,7 +6176,7 @@
         <v>39</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="27">
         <v>95</v>
@@ -6161,12 +6185,12 @@
         <v>10273</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="36" t="s">
         <v>14</v>
@@ -6175,7 +6199,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F29" s="27">
         <v>95</v>
@@ -6184,12 +6208,12 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" s="36" t="s">
         <v>14</v>
@@ -6198,7 +6222,7 @@
         <v>39</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F30" s="27">
         <v>95</v>
@@ -6207,12 +6231,12 @@
         <v>436</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C31" s="36" t="s">
         <v>14</v>
@@ -6221,7 +6245,7 @@
         <v>39</v>
       </c>
       <c r="E31" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F31" s="27">
         <v>437</v>
@@ -6230,12 +6254,12 @@
         <v>934</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C32" s="36" t="s">
         <v>14</v>
@@ -6244,7 +6268,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F32" s="27">
         <v>935</v>
@@ -6253,12 +6277,12 @@
         <v>2419</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="36" t="s">
         <v>14</v>
@@ -6267,7 +6291,7 @@
         <v>39</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F33" s="27">
         <v>2420</v>
@@ -6276,12 +6300,12 @@
         <v>10270</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="36" t="s">
         <v>14</v>
@@ -6299,12 +6323,12 @@
         <v>3475</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" s="36" t="s">
         <v>14</v>
@@ -6313,7 +6337,7 @@
         <v>39</v>
       </c>
       <c r="E35" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F35" s="27">
         <v>3476</v>
@@ -6322,12 +6346,12 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B36" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C36" s="36" t="s">
         <v>14</v>
@@ -6336,7 +6360,7 @@
         <v>39</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F36" s="27">
         <v>4130</v>
@@ -6345,12 +6369,12 @@
         <v>4519</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C37" s="36" t="s">
         <v>14</v>
@@ -6368,12 +6392,12 @@
         <v>6376</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="36" t="s">
         <v>14</v>
@@ -6382,7 +6406,7 @@
         <v>39</v>
       </c>
       <c r="E38" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F38" s="27">
         <v>6377</v>
@@ -6391,12 +6415,12 @@
         <v>6757</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="36" t="s">
         <v>14</v>
@@ -6414,12 +6438,12 @@
         <v>6826</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C40" s="36" t="s">
         <v>14</v>
@@ -6428,7 +6452,7 @@
         <v>39</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F40" s="27">
         <v>7574</v>
@@ -6437,12 +6461,12 @@
         <v>10270</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="36" t="s">
         <v>29</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="36" t="s">
         <v>14</v>
@@ -6460,12 +6484,12 @@
         <v>10735</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" s="37" t="s">
         <v>14</v>
@@ -6474,7 +6498,7 @@
         <v>41</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F42" s="7">
         <v>1</v>
@@ -6483,12 +6507,12 @@
         <v>10862</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="16" customHeight="1">
+    <row r="43" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" s="37" t="s">
         <v>14</v>
@@ -6506,12 +6530,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B44" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C44" s="37" t="s">
         <v>14</v>
@@ -6520,7 +6544,7 @@
         <v>41</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" s="7">
         <v>119</v>
@@ -6529,12 +6553,12 @@
         <v>10354</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B45" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C45" s="37" t="s">
         <v>14</v>
@@ -6543,7 +6567,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F45" s="7">
         <v>119</v>
@@ -6552,12 +6576,12 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C46" s="37" t="s">
         <v>14</v>
@@ -6566,7 +6590,7 @@
         <v>41</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F46" s="7">
         <v>119</v>
@@ -6575,12 +6599,12 @@
         <v>481</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C47" s="37" t="s">
         <v>14</v>
@@ -6589,7 +6613,7 @@
         <v>41</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F47" s="7">
         <v>482</v>
@@ -6598,12 +6622,12 @@
         <v>973</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C48" s="37" t="s">
         <v>14</v>
@@ -6612,7 +6636,7 @@
         <v>41</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F48" s="7">
         <v>974</v>
@@ -6621,12 +6645,12 @@
         <v>2452</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="37" t="s">
         <v>14</v>
@@ -6635,7 +6659,7 @@
         <v>41</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F49" s="7">
         <v>2453</v>
@@ -6644,12 +6668,12 @@
         <v>10351</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="37" t="s">
         <v>14</v>
@@ -6667,12 +6691,12 @@
         <v>3508</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="37" t="s">
         <v>14</v>
@@ -6681,7 +6705,7 @@
         <v>41</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F51" s="7">
         <v>3509</v>
@@ -6690,12 +6714,12 @@
         <v>4180</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52" s="37" t="s">
         <v>14</v>
@@ -6704,7 +6728,7 @@
         <v>41</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F52" s="7">
         <v>4181</v>
@@ -6713,12 +6737,12 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="37" t="s">
         <v>14</v>
@@ -6736,12 +6760,12 @@
         <v>6439</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B54" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C54" s="37" t="s">
         <v>14</v>
@@ -6750,7 +6774,7 @@
         <v>41</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F54" s="7">
         <v>6440</v>
@@ -6759,12 +6783,12 @@
         <v>6817</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B55" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C55" s="37" t="s">
         <v>14</v>
@@ -6782,12 +6806,12 @@
         <v>6886</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C56" s="37" t="s">
         <v>14</v>
@@ -6796,7 +6820,7 @@
         <v>41</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F56" s="7">
         <v>6887</v>
@@ -6805,12 +6829,12 @@
         <v>7636</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B57" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57" s="37" t="s">
         <v>14</v>
@@ -6828,12 +6852,12 @@
         <v>10351</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B58" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C58" s="37" t="s">
         <v>14</v>
@@ -6851,21 +6875,21 @@
         <v>10862</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="37" t="s">
         <v>48</v>
       </c>
       <c r="B59" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="39" t="s">
         <v>14</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F59" s="9">
         <v>1</v>
@@ -6874,21 +6898,21 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="37" t="s">
         <v>48</v>
       </c>
       <c r="B60" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C60" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="C60" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="F60" s="9">
         <v>1</v>
@@ -6897,12 +6921,12 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="37" t="s">
         <v>51</v>
       </c>
       <c r="B61" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C61" s="39" t="s">
         <v>14</v>
@@ -6911,7 +6935,7 @@
         <v>50</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F61" s="1">
         <v>1</v>
@@ -6920,12 +6944,12 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="37" t="s">
         <v>51</v>
       </c>
       <c r="B62" s="37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C62" s="39" t="s">
         <v>14</v>
@@ -6934,7 +6958,7 @@
         <v>50</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F62" s="1">
         <v>1</v>
@@ -6943,12 +6967,12 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" s="36" t="s">
         <v>14</v>
@@ -6957,7 +6981,7 @@
         <v>43</v>
       </c>
       <c r="E63" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F63" s="27">
         <v>1</v>
@@ -6966,12 +6990,12 @@
         <v>10839</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C64" s="36" t="s">
         <v>14</v>
@@ -6989,12 +7013,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C65" s="36" t="s">
         <v>14</v>
@@ -7003,7 +7027,7 @@
         <v>43</v>
       </c>
       <c r="E65" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F65" s="27">
         <v>112</v>
@@ -7012,12 +7036,12 @@
         <v>10359</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66" s="36" t="s">
         <v>14</v>
@@ -7026,7 +7050,7 @@
         <v>43</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F66" s="27">
         <v>112</v>
@@ -7035,12 +7059,12 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>14</v>
@@ -7049,7 +7073,7 @@
         <v>43</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F67" s="27">
         <v>112</v>
@@ -7058,12 +7082,12 @@
         <v>441</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B68" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" s="36" t="s">
         <v>14</v>
@@ -7072,7 +7096,7 @@
         <v>43</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F68" s="27">
         <v>442</v>
@@ -7081,12 +7105,12 @@
         <v>945</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C69" s="36" t="s">
         <v>14</v>
@@ -7095,7 +7119,7 @@
         <v>43</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F69" s="27">
         <v>946</v>
@@ -7104,12 +7128,12 @@
         <v>2436</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C70" s="36" t="s">
         <v>14</v>
@@ -7118,7 +7142,7 @@
         <v>43</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F70" s="27">
         <v>2437</v>
@@ -7127,12 +7151,12 @@
         <v>10356</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B71" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C71" s="36" t="s">
         <v>14</v>
@@ -7150,12 +7174,12 @@
         <v>3495</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B72" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C72" s="36" t="s">
         <v>14</v>
@@ -7164,7 +7188,7 @@
         <v>43</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F72" s="27">
         <v>3496</v>
@@ -7173,12 +7197,12 @@
         <v>4185</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B73" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C73" s="36" t="s">
         <v>14</v>
@@ -7187,7 +7211,7 @@
         <v>43</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F73" s="27">
         <v>4186</v>
@@ -7196,12 +7220,12 @@
         <v>4578</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B74" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C74" s="36" t="s">
         <v>14</v>
@@ -7219,12 +7243,12 @@
         <v>6444</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B75" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C75" s="36" t="s">
         <v>14</v>
@@ -7233,7 +7257,7 @@
         <v>43</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F75" s="27">
         <v>6445</v>
@@ -7242,12 +7266,12 @@
         <v>6822</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B76" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C76" s="36" t="s">
         <v>14</v>
@@ -7265,12 +7289,12 @@
         <v>6891</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B77" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C77" s="36" t="s">
         <v>14</v>
@@ -7279,7 +7303,7 @@
         <v>43</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F77" s="27">
         <v>6892</v>
@@ -7288,12 +7312,12 @@
         <v>7647</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B78" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C78" s="36" t="s">
         <v>14</v>
@@ -7311,12 +7335,12 @@
         <v>10356</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="36" t="s">
         <v>33</v>
       </c>
       <c r="B79" s="36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C79" s="36" t="s">
         <v>14</v>
@@ -7334,21 +7358,21 @@
         <v>10839</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C80" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D80" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F80" s="27">
         <v>1</v>
@@ -7357,18 +7381,18 @@
         <v>9646</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C81" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D81" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E81" s="27" t="s">
         <v>15</v>
@@ -7380,21 +7404,21 @@
         <v>341</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C82" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D82" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F82" s="27">
         <v>342</v>
@@ -7403,21 +7427,21 @@
         <v>9377</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C83" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D83" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F83" s="27">
         <v>342</v>
@@ -7426,18 +7450,18 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C84" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D84" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E84" s="27" t="s">
         <v>22</v>
@@ -7449,21 +7473,21 @@
         <v>914</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C85" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D85" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F85" s="27">
         <v>915</v>
@@ -7472,21 +7496,21 @@
         <v>1490</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C86" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D86" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F86" s="27">
         <v>1491</v>
@@ -7495,21 +7519,21 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C87" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D87" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E87" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F87" s="27">
         <v>2580</v>
@@ -7518,21 +7542,21 @@
         <v>9374</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C88" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D88" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E88" s="27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F88" s="27">
         <v>2580</v>
@@ -7541,21 +7565,21 @@
         <v>2768</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C89" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D89" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E89" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F89" s="27">
         <v>2769</v>
@@ -7564,18 +7588,18 @@
         <v>3419</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C90" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D90" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E90" s="27" t="s">
         <v>7</v>
@@ -7587,21 +7611,21 @@
         <v>5312</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C91" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D91" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E91" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F91" s="27">
         <v>5313</v>
@@ -7610,21 +7634,21 @@
         <v>5474</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C92" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D92" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E92" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F92" s="27">
         <v>5475</v>
@@ -7633,18 +7657,18 @@
         <v>6257</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C93" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D93" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E93" s="27" t="s">
         <v>24</v>
@@ -7656,18 +7680,18 @@
         <v>7601</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C94" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D94" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E94" s="27" t="s">
         <v>25</v>
@@ -7679,18 +7703,18 @@
         <v>9374</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C95" s="31" t="s">
         <v>21</v>
       </c>
       <c r="D95" s="40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E95" s="27" t="s">
         <v>11</v>
@@ -7702,19 +7726,19 @@
         <v>9646</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B96" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C96" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D96"/>
       <c r="E96" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F96" s="27">
         <v>1</v>
@@ -7723,12 +7747,12 @@
         <v>9867</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B97" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C97" s="35" t="s">
         <v>26</v>
@@ -7744,19 +7768,19 @@
         <v>327</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B98" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C98" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D98"/>
       <c r="E98" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F98" s="27">
         <v>328</v>
@@ -7765,19 +7789,19 @@
         <v>9501</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B99" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C99" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D99"/>
       <c r="E99" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F99" s="27">
         <v>328</v>
@@ -7786,19 +7810,19 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B100" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C100" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D100"/>
       <c r="E100" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F100" s="27">
         <v>328</v>
@@ -7807,19 +7831,19 @@
         <v>564</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B101" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C101" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D101"/>
       <c r="E101" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F101" s="27">
         <v>565</v>
@@ -7828,19 +7852,19 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B102" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C102" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D102"/>
       <c r="E102" s="27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F102" s="27">
         <v>1138</v>
@@ -7849,19 +7873,19 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B103" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C103" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D103"/>
       <c r="E103" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F103" s="27">
         <v>2200</v>
@@ -7870,19 +7894,19 @@
         <v>2910</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B104" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C104" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D104"/>
       <c r="E104" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F104" s="27">
         <v>2911</v>
@@ -7891,19 +7915,19 @@
         <v>9498</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B105" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C105" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D105"/>
       <c r="E105" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F105" s="27">
         <v>2911</v>
@@ -7912,12 +7936,12 @@
         <v>3630</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B106" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C106" s="35" t="s">
         <v>26</v>
@@ -7933,19 +7957,19 @@
         <v>5514</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B107" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C107" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D107"/>
       <c r="E107" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F107" s="27">
         <v>5515</v>
@@ -7954,19 +7978,19 @@
         <v>5637</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B108" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C108" s="35" t="s">
         <v>26</v>
       </c>
       <c r="D108"/>
       <c r="E108" s="27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F108" s="27">
         <v>5638</v>
@@ -7975,12 +7999,12 @@
         <v>6423</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B109" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C109" s="35" t="s">
         <v>26</v>
@@ -7996,12 +8020,12 @@
         <v>7797</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B110" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C110" s="35" t="s">
         <v>26</v>
@@ -8017,12 +8041,12 @@
         <v>9498</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" s="35" t="s">
         <v>37</v>
       </c>
       <c r="B111" s="35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C111" s="35" t="s">
         <v>26</v>
@@ -8038,21 +8062,21 @@
         <v>9867</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>54</v>
       </c>
       <c r="B112" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C112" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D112" s="22" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F112" s="27">
         <v>1</v>
@@ -8061,18 +8085,18 @@
         <v>19199</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>54</v>
       </c>
       <c r="B113" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C113" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D113" s="22" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="E113" s="27" t="s">
         <v>15</v>
@@ -8084,21 +8108,21 @@
         <v>350</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>54</v>
       </c>
       <c r="B114" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C114" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D114" s="22" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F114" s="27">
         <v>351</v>
@@ -8107,18 +8131,18 @@
         <v>18068</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>54</v>
       </c>
       <c r="B115" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C115" s="16" t="s">
         <v>55</v>
       </c>
       <c r="D115" s="22" t="s">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="E115" s="27" t="s">
         <v>11</v>
@@ -8130,19 +8154,21 @@
         <v>19199</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B116" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B116" s="32" t="s">
+      <c r="C116" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C116" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="D116" s="6"/>
+      <c r="D116" s="27" t="s">
+        <v>111</v>
+      </c>
       <c r="E116" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F116" s="27">
         <v>1</v>
@@ -8151,15 +8177,18 @@
         <v>18554</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B117" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B117" s="32" t="s">
+      <c r="C117" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C117" s="33" t="s">
-        <v>87</v>
+      <c r="D117" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="E117" s="27" t="s">
         <v>15</v>
@@ -8171,18 +8200,21 @@
         <v>199</v>
       </c>
     </row>
-    <row r="118" spans="1:7">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B118" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B118" s="32" t="s">
+      <c r="C118" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C118" s="33" t="s">
-        <v>87</v>
+      <c r="D118" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="E118" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F118" s="27">
         <v>200</v>
@@ -8191,15 +8223,18 @@
         <v>17905</v>
       </c>
     </row>
-    <row r="119" spans="1:7">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B119" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B119" s="32" t="s">
+      <c r="C119" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C119" s="33" t="s">
-        <v>87</v>
+      <c r="D119" s="27" t="s">
+        <v>111</v>
       </c>
       <c r="E119" s="27" t="s">
         <v>11</v>
@@ -8211,19 +8246,19 @@
         <v>18554</v>
       </c>
     </row>
-    <row r="120" spans="1:7">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B120" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C120" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D120" s="27"/>
       <c r="E120" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F120" s="27">
         <v>1</v>
@@ -8232,12 +8267,12 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="121" spans="1:7">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B121" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>27</v>
@@ -8253,19 +8288,19 @@
         <v>385</v>
       </c>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B122" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C122" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D122" s="27"/>
       <c r="E122" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F122" s="27">
         <v>386</v>
@@ -8274,19 +8309,19 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B123" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C123" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D123" s="27"/>
       <c r="E123" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F123" s="27">
         <v>386</v>
@@ -8295,19 +8330,19 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="124" spans="1:7">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B124" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C124" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D124" s="27"/>
       <c r="E124" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F124" s="27">
         <v>386</v>
@@ -8316,19 +8351,19 @@
         <v>889</v>
       </c>
     </row>
-    <row r="125" spans="1:7">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B125" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C125" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D125" s="27"/>
       <c r="E125" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F125" s="27">
         <v>890</v>
@@ -8337,12 +8372,12 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="126" spans="1:7">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B126" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C126" s="30" t="s">
         <v>27</v>
@@ -8358,19 +8393,19 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="127" spans="1:7">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B127" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C127" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D127" s="27"/>
       <c r="E127" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F127" s="27">
         <v>1877</v>
@@ -8379,19 +8414,19 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="128" spans="1:7">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B128" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C128" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D128" s="27"/>
       <c r="E128" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F128" s="27">
         <v>2462</v>
@@ -8400,19 +8435,19 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="129" spans="1:7">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B129" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C129" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D129" s="27"/>
       <c r="E129" s="27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F129" s="27">
         <v>3584</v>
@@ -8421,12 +8456,12 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B130" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C130" s="30" t="s">
         <v>27</v>
@@ -8442,19 +8477,19 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B131" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C131" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D131" s="27"/>
       <c r="E131" s="27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F131" s="27">
         <v>7472</v>
@@ -8463,19 +8498,19 @@
         <v>7663</v>
       </c>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B132" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C132" s="30" t="s">
         <v>27</v>
       </c>
       <c r="D132" s="27"/>
       <c r="E132" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F132" s="27">
         <v>7664</v>
@@ -8484,12 +8519,12 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="133" spans="1:7">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B133" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C133" s="30" t="s">
         <v>27</v>
@@ -8505,12 +8540,12 @@
         <v>10192</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B134" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C134" s="30" t="s">
         <v>27</v>
@@ -8526,12 +8561,12 @@
         <v>12349</v>
       </c>
     </row>
-    <row r="135" spans="1:7">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B135" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C135" s="30" t="s">
         <v>27</v>
@@ -8547,19 +8582,19 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="136" spans="1:7">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B136" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C136" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D136" s="27"/>
       <c r="E136" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F136" s="27">
         <v>1</v>
@@ -8568,19 +8603,19 @@
         <v>10053</v>
       </c>
     </row>
-    <row r="137" spans="1:7">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B137" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C137" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D137" s="27"/>
       <c r="E137" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F137" s="27">
         <v>1</v>
@@ -8589,19 +8624,19 @@
         <v>10053</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B138" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C138" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D138" s="27"/>
       <c r="E138" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F138" s="27">
         <v>1</v>
@@ -8610,19 +8645,19 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B139" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C139" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D139" s="27"/>
       <c r="E139" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F139" s="27">
         <v>1</v>
@@ -8631,19 +8666,19 @@
         <v>345</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B140" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C140" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D140" s="27"/>
       <c r="E140" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F140" s="27">
         <v>346</v>
@@ -8652,19 +8687,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="141" spans="1:7">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B141" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C141" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D141" s="27"/>
       <c r="E141" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F141" s="27">
         <v>655</v>
@@ -8673,19 +8708,19 @@
         <v>852</v>
       </c>
     </row>
-    <row r="142" spans="1:7">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B142" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C142" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D142" s="27"/>
       <c r="E142" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F142" s="27">
         <v>853</v>
@@ -8694,19 +8729,19 @@
         <v>2358</v>
       </c>
     </row>
-    <row r="143" spans="1:7">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B143" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C143" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D143" s="27"/>
       <c r="E143" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F143" s="27">
         <v>2359</v>
@@ -8715,15 +8750,15 @@
         <v>10050</v>
       </c>
     </row>
-    <row r="144" spans="1:7">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B144" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C144" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D144" s="27"/>
       <c r="E144" s="27" t="s">
@@ -8736,19 +8771,19 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B145" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C145" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D145" s="27"/>
       <c r="E145" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F145" s="27">
         <v>3391</v>
@@ -8757,19 +8792,19 @@
         <v>3978</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B146" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C146" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D146" s="27"/>
       <c r="E146" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F146" s="27">
         <v>3979</v>
@@ -8778,15 +8813,15 @@
         <v>4431</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B147" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C147" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D147" s="27"/>
       <c r="E147" s="27" t="s">
@@ -8799,19 +8834,19 @@
         <v>6303</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B148" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C148" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D148" s="27"/>
       <c r="E148" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F148" s="27">
         <v>6304</v>
@@ -8820,15 +8855,15 @@
         <v>6687</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B149" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C149" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D149" s="27"/>
       <c r="E149" s="27" t="s">
@@ -8841,19 +8876,19 @@
         <v>6762</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B150" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C150" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D150" s="27"/>
       <c r="E150" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F150" s="27">
         <v>6763</v>
@@ -8862,15 +8897,15 @@
         <v>7557</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="27" t="s">
         <v>52</v>
       </c>
       <c r="B151" s="27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C151" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D151" s="27"/>
       <c r="E151" s="27" t="s">
@@ -8884,339 +8919,385 @@
       </c>
       <c r="H151" s="25"/>
     </row>
-    <row r="193" spans="2:4">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B152" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C152" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D152" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E152" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F152" s="27">
+        <v>105</v>
+      </c>
+      <c r="G152" s="27">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>113</v>
+      </c>
+      <c r="B153" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C153" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="D153" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E153" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F153" s="27">
+        <v>117</v>
+      </c>
+      <c r="G153" s="27">
+        <v>2543</v>
+      </c>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B193" s="1"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5"/>
     </row>
-    <row r="194" spans="2:4">
+    <row r="194" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B194" s="1"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5"/>
     </row>
-    <row r="195" spans="2:4">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B195" s="1"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5"/>
     </row>
-    <row r="196" spans="2:4">
+    <row r="196" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B196" s="1"/>
       <c r="C196" s="5"/>
       <c r="D196" s="5"/>
     </row>
-    <row r="197" spans="2:4">
+    <row r="197" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B197" s="1"/>
       <c r="C197" s="5"/>
       <c r="D197" s="5"/>
     </row>
-    <row r="198" spans="2:4">
+    <row r="198" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B198" s="1"/>
       <c r="C198" s="5"/>
       <c r="D198" s="5"/>
     </row>
-    <row r="199" spans="2:4">
+    <row r="199" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B199" s="1"/>
       <c r="C199" s="5"/>
       <c r="D199" s="5"/>
     </row>
-    <row r="200" spans="2:4">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B200" s="1"/>
       <c r="C200" s="5"/>
       <c r="D200" s="5"/>
     </row>
-    <row r="201" spans="2:4">
+    <row r="201" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B201" s="1"/>
       <c r="C201" s="5"/>
       <c r="D201" s="5"/>
     </row>
-    <row r="202" spans="2:4">
+    <row r="202" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B202" s="1"/>
       <c r="C202" s="5"/>
       <c r="D202" s="5"/>
     </row>
-    <row r="203" spans="2:4">
+    <row r="203" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B203" s="1"/>
       <c r="C203" s="5"/>
       <c r="D203" s="5"/>
     </row>
-    <row r="204" spans="2:4">
+    <row r="204" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B204" s="1"/>
       <c r="C204" s="5"/>
       <c r="D204" s="5"/>
     </row>
-    <row r="205" spans="2:4">
+    <row r="205" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B205" s="1"/>
       <c r="C205" s="5"/>
       <c r="D205" s="5"/>
     </row>
-    <row r="206" spans="2:4">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B206" s="1"/>
       <c r="C206" s="5"/>
       <c r="D206" s="5"/>
     </row>
-    <row r="207" spans="2:4">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B207" s="1"/>
       <c r="C207" s="5"/>
       <c r="D207" s="5"/>
     </row>
-    <row r="208" spans="2:4">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B208" s="1"/>
       <c r="C208" s="5"/>
       <c r="D208" s="5"/>
     </row>
-    <row r="209" spans="2:4">
+    <row r="209" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B209" s="1"/>
       <c r="C209" s="5"/>
       <c r="D209" s="5"/>
     </row>
-    <row r="210" spans="2:4">
+    <row r="210" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B210" s="1"/>
       <c r="C210" s="5"/>
       <c r="D210" s="5"/>
     </row>
-    <row r="211" spans="2:4">
+    <row r="211" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B211" s="1"/>
       <c r="C211" s="5"/>
       <c r="D211" s="5"/>
     </row>
-    <row r="212" spans="2:4">
+    <row r="212" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B212" s="1"/>
       <c r="C212" s="5"/>
       <c r="D212" s="5"/>
     </row>
-    <row r="213" spans="2:4">
+    <row r="213" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B213" s="1"/>
       <c r="C213" s="5"/>
       <c r="D213" s="5"/>
     </row>
-    <row r="214" spans="2:4">
+    <row r="214" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B214" s="1"/>
       <c r="C214" s="5"/>
       <c r="D214" s="5"/>
     </row>
-    <row r="215" spans="2:4">
+    <row r="215" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B215" s="1"/>
       <c r="C215" s="5"/>
       <c r="D215" s="5"/>
     </row>
-    <row r="216" spans="2:4">
+    <row r="216" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B216" s="1"/>
       <c r="C216" s="5"/>
       <c r="D216" s="5"/>
     </row>
-    <row r="217" spans="2:4">
+    <row r="217" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B217" s="1"/>
     </row>
-    <row r="218" spans="2:4">
+    <row r="218" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B218" s="1"/>
       <c r="C218" s="5"/>
       <c r="D218" s="5"/>
     </row>
-    <row r="219" spans="2:4">
+    <row r="219" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B219" s="1"/>
       <c r="C219" s="5"/>
       <c r="D219" s="5"/>
     </row>
-    <row r="220" spans="2:4">
+    <row r="220" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B220" s="1"/>
       <c r="C220" s="5"/>
       <c r="D220" s="5"/>
     </row>
-    <row r="221" spans="2:4">
+    <row r="221" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B221" s="1"/>
       <c r="C221" s="5"/>
       <c r="D221" s="5"/>
     </row>
-    <row r="222" spans="2:4">
+    <row r="222" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B222" s="1"/>
       <c r="C222" s="5"/>
       <c r="D222" s="5"/>
     </row>
-    <row r="223" spans="2:4">
+    <row r="223" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B223" s="1"/>
       <c r="C223" s="5"/>
       <c r="D223" s="5"/>
     </row>
-    <row r="224" spans="2:4">
+    <row r="224" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B224" s="1"/>
       <c r="C224" s="5"/>
       <c r="D224" s="5"/>
     </row>
-    <row r="907" spans="5:5">
+    <row r="907" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E907" s="1"/>
     </row>
-    <row r="1043" spans="2:2">
+    <row r="1043" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1043" s="1"/>
     </row>
-    <row r="1044" spans="2:2">
+    <row r="1044" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1044" s="1"/>
     </row>
-    <row r="1169" spans="2:2">
+    <row r="1169" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1169" s="1"/>
     </row>
-    <row r="1170" spans="2:2">
+    <row r="1170" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1170" s="1"/>
     </row>
-    <row r="1171" spans="2:2">
+    <row r="1171" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1171" s="1"/>
     </row>
-    <row r="1172" spans="2:2">
+    <row r="1172" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1172" s="1"/>
     </row>
-    <row r="1173" spans="2:2">
+    <row r="1173" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1173" s="1"/>
     </row>
-    <row r="1174" spans="2:2">
+    <row r="1174" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1174" s="1"/>
     </row>
-    <row r="1219" spans="2:6">
+    <row r="1219" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1219" s="1"/>
       <c r="F1219" s="1"/>
     </row>
-    <row r="1220" spans="2:6">
+    <row r="1220" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1220" s="1"/>
       <c r="F1220" s="1"/>
     </row>
-    <row r="1221" spans="2:6">
+    <row r="1221" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E1221" s="1"/>
       <c r="F1221" s="1"/>
     </row>
-    <row r="1223" spans="2:6">
+    <row r="1223" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1223" s="1"/>
     </row>
-    <row r="1224" spans="2:6">
+    <row r="1224" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1224" s="1"/>
     </row>
-    <row r="1225" spans="2:6">
+    <row r="1225" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1225" s="1"/>
     </row>
-    <row r="1226" spans="2:6">
+    <row r="1226" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1226" s="1"/>
     </row>
-    <row r="1227" spans="2:6">
+    <row r="1227" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B1227" s="1"/>
     </row>
-    <row r="1246" spans="2:2">
+    <row r="1246" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1246" s="1"/>
     </row>
-    <row r="1247" spans="2:2">
+    <row r="1247" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1247" s="1"/>
     </row>
-    <row r="1248" spans="2:2">
+    <row r="1248" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1248" s="1"/>
     </row>
-    <row r="1249" spans="2:2">
+    <row r="1249" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1249" s="1"/>
     </row>
-    <row r="1250" spans="2:2">
+    <row r="1250" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1250" s="1"/>
     </row>
-    <row r="1251" spans="2:2">
+    <row r="1251" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1251" s="1"/>
     </row>
-    <row r="1252" spans="2:2">
+    <row r="1252" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1252" s="1"/>
     </row>
-    <row r="1254" spans="2:2">
+    <row r="1254" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1254" s="1"/>
     </row>
-    <row r="1255" spans="2:2">
+    <row r="1255" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1255" s="1"/>
     </row>
-    <row r="1256" spans="2:2">
+    <row r="1256" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1256" s="1"/>
     </row>
-    <row r="1257" spans="2:2">
+    <row r="1257" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1257" s="1"/>
     </row>
-    <row r="1258" spans="2:2">
+    <row r="1258" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1258" s="1"/>
     </row>
-    <row r="1259" spans="2:2">
+    <row r="1259" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1259" s="1"/>
     </row>
-    <row r="1311" spans="2:2">
+    <row r="1311" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1311" s="1"/>
     </row>
-    <row r="1312" spans="2:2">
+    <row r="1312" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1312" s="1"/>
     </row>
-    <row r="1313" spans="2:2">
+    <row r="1313" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1313" s="1"/>
     </row>
-    <row r="1314" spans="2:2">
+    <row r="1314" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1314" s="1"/>
     </row>
-    <row r="1316" spans="2:2">
+    <row r="1316" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1316" s="1"/>
     </row>
-    <row r="1317" spans="2:2">
+    <row r="1317" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1317" s="1"/>
     </row>
-    <row r="1318" spans="2:2">
+    <row r="1318" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1318" s="1"/>
     </row>
-    <row r="1319" spans="2:2">
+    <row r="1319" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1319" s="1"/>
     </row>
-    <row r="1354" spans="2:2">
+    <row r="1354" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1354" s="1"/>
     </row>
-    <row r="1355" spans="2:2">
+    <row r="1355" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1355" s="1"/>
     </row>
-    <row r="1356" spans="2:2">
+    <row r="1356" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1356" s="1"/>
     </row>
-    <row r="1357" spans="2:2">
+    <row r="1357" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1357" s="1"/>
     </row>
-    <row r="1358" spans="2:2">
+    <row r="1358" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1358" s="1"/>
     </row>
-    <row r="1359" spans="2:2">
+    <row r="1359" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1359" s="1"/>
     </row>
-    <row r="1401" spans="3:6">
+    <row r="1401" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1401" s="1"/>
       <c r="F1401" s="1"/>
     </row>
-    <row r="1402" spans="3:6">
+    <row r="1402" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1402" s="6"/>
       <c r="D1402" s="6"/>
       <c r="E1402" s="1"/>
       <c r="F1402" s="1"/>
     </row>
-    <row r="1403" spans="3:6">
+    <row r="1403" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1403" s="6"/>
       <c r="D1403" s="6"/>
       <c r="E1403" s="1"/>
       <c r="F1403" s="1"/>
     </row>
-    <row r="1404" spans="3:6">
+    <row r="1404" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C1404" s="6"/>
       <c r="D1404" s="6"/>
       <c r="E1404" s="1"/>
       <c r="F1404" s="1"/>
     </row>
-    <row r="1405" spans="3:6">
+    <row r="1405" spans="3:6" x14ac:dyDescent="0.2">
       <c r="E1405" s="1"/>
       <c r="F1405" s="1"/>
     </row>
-    <row r="1468" spans="2:2">
+    <row r="1468" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1468" s="1"/>
     </row>
-    <row r="1469" spans="2:2">
+    <row r="1469" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1469" s="1"/>
     </row>
-    <row r="1470" spans="2:2">
+    <row r="1470" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1470" s="1"/>
     </row>
-    <row r="1471" spans="2:2">
+    <row r="1471" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B1471" s="1"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G1456">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G1456">
     <sortCondition ref="C2:C1456"/>
     <sortCondition ref="D2:D1456"/>
   </sortState>
@@ -9231,16 +9312,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G43" sqref="A28:G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -9263,7 +9344,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -9286,7 +9367,7 @@
         <v>10389</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -9309,7 +9390,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -9332,7 +9413,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -9355,7 +9436,7 @@
         <v>2457</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -9378,7 +9459,7 @@
         <v>3513</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9401,7 +9482,7 @@
         <v>4206</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -9424,7 +9505,7 @@
         <v>4599</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -9447,7 +9528,7 @@
         <v>6456</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -9470,7 +9551,7 @@
         <v>6903</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -9493,7 +9574,7 @@
         <v>7671</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -9516,7 +9597,7 @@
         <v>10386</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -9539,7 +9620,7 @@
         <v>10962</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -9562,7 +9643,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -9585,7 +9666,7 @@
         <v>10366</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -9608,7 +9689,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -9631,7 +9712,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -9654,7 +9735,7 @@
         <v>2476</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -9677,7 +9758,7 @@
         <v>3532</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -9700,7 +9781,7 @@
         <v>4210</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="14" customHeight="1">
+    <row r="21" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -9723,7 +9804,7 @@
         <v>4600</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -9746,7 +9827,7 @@
         <v>6451</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -9769,7 +9850,7 @@
         <v>6832</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -9792,7 +9873,7 @@
         <v>6901</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -9815,7 +9896,7 @@
         <v>7654</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -9838,7 +9919,7 @@
         <v>10363</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -9861,21 +9942,21 @@
         <v>10794</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>48</v>
       </c>
       <c r="B28" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>70</v>
-      </c>
-      <c r="C28" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>71</v>
       </c>
       <c r="F28" s="9">
         <v>1</v>
@@ -9884,12 +9965,12 @@
         <v>10116</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>51</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>14</v>
@@ -9898,7 +9979,7 @@
         <v>50</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -9907,12 +9988,12 @@
         <v>10242</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" t="s">
         <v>27</v>
@@ -9927,18 +10008,18 @@
         <v>385</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="10">
         <v>386</v>
@@ -9947,18 +10028,18 @@
         <v>12352</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F32" s="9">
         <v>386</v>
@@ -9967,12 +10048,12 @@
         <v>889</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
         <v>27</v>
@@ -9987,12 +10068,12 @@
         <v>1195</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
         <v>27</v>
@@ -10007,18 +10088,18 @@
         <v>1876</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
         <v>27</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="9">
         <v>1877</v>
@@ -10027,18 +10108,18 @@
         <v>2461</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F36" s="9">
         <v>2462</v>
@@ -10047,12 +10128,12 @@
         <v>3583</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
@@ -10067,12 +10148,12 @@
         <v>3793</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
         <v>27</v>
@@ -10087,12 +10168,12 @@
         <v>7471</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>35</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
         <v>27</v>
@@ -10107,12 +10188,12 @@
         <v>7663</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
         <v>27</v>
@@ -10127,12 +10208,12 @@
         <v>8704</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
         <v>27</v>
@@ -10147,12 +10228,12 @@
         <v>10192</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
         <v>27</v>
@@ -10167,12 +10248,12 @@
         <v>12349</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
         <v>27</v>
@@ -10187,12 +10268,12 @@
         <v>12573</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
         <v>49</v>
@@ -10210,12 +10291,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
         <v>49</v>
@@ -10233,12 +10314,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
         <v>49</v>
@@ -10247,7 +10328,7 @@
         <v>49</v>
       </c>
       <c r="E46" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F46">
         <v>105</v>
@@ -10256,12 +10337,12 @@
         <v>2849</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" t="s">
         <v>49</v>

</xml_diff>